<commit_message>
major revision of model and source files, updates to csv editor and results viewer, added policies, renamed sector files, updated Reference.ipynb
</commit_message>
<xml_diff>
--- a/csv/model/CIMS_base/formula_CIMS_base_AB.xlsx
+++ b/csv/model/CIMS_base/formula_CIMS_base_AB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\CIMS_base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CIMS\dev\cims-models\csv\model\CIMS_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFD03DC2-A2BB-4DFD-AA19-29BB9516E724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36543896-C053-4CF5-BDDB-A404AE512B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40980" yWindow="4095" windowWidth="17280" windowHeight="8880" xr2:uid="{D4FDFC50-15E1-4CA4-93A0-790CA34B4E5C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14724549-7B89-4625-AD24-6A4785BB65F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="191029" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,6 +36,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -192,13 +214,15 @@
       <sheetName val="Prices"/>
       <sheetName val="Carbon_tax"/>
       <sheetName val="Demand"/>
+      <sheetName val="Elec markups"/>
+      <sheetName val="CER"/>
       <sheetName val="Conversions"/>
       <sheetName val="Coefficients"/>
     </sheetNames>
     <definedNames>
-      <definedName name="pyCIMS_GDP" refersTo="='Macro'!$D$59:$R$74"/>
-      <definedName name="pyCIMS_population" refersTo="='Macro'!$D$4:$R$19"/>
-      <definedName name="pyCIMS_year" refersTo="='Macro'!$D$1:$R$1"/>
+      <definedName name="CIMS_GDP" refersTo="='Macro'!$D$59:$R$74"/>
+      <definedName name="CIMS_population" refersTo="='Macro'!$D$4:$R$19"/>
+      <definedName name="CIMS_year" refersTo="='Macro'!$D$1:$R$1"/>
       <definedName name="region_CIMS" refersTo="='Control'!$B$19:$B$34"/>
     </definedNames>
     <sheetDataSet>
@@ -299,6 +323,51 @@
             <v>TR</v>
           </cell>
         </row>
+        <row r="59">
+          <cell r="D59" t="str">
+            <v>Industrial</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="D60" t="str">
+            <v>Commercial</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="D61" t="str">
+            <v>Industrial</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="D64" t="str">
+            <v>CER fuels</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="D65" t="str">
+            <v>Electricity</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="D66" t="str">
+            <v>Natural Gas</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="D67" t="str">
+            <v>Fuel Oil</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="D68" t="str">
+            <v>Gasoline</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="D69" t="str">
+            <v>Diesel</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="1">
@@ -1750,666 +1819,6 @@
             <v>2035</v>
           </cell>
         </row>
-        <row r="4">
-          <cell r="D4" t="str">
-            <v>Brent</v>
-          </cell>
-          <cell r="E4" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F4">
-            <v>2020</v>
-          </cell>
-          <cell r="G4" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H4" t="str">
-            <v>bbl</v>
-          </cell>
-          <cell r="I4" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K4">
-            <v>77.624814851455724</v>
-          </cell>
-          <cell r="L4">
-            <v>77.624814851455724</v>
-          </cell>
-          <cell r="M4">
-            <v>101.39911303920623</v>
-          </cell>
-          <cell r="N4">
-            <v>60.837965156576949</v>
-          </cell>
-          <cell r="O4">
-            <v>72.811378070272852</v>
-          </cell>
-          <cell r="P4">
-            <v>75.993051453005904</v>
-          </cell>
-          <cell r="Q4">
-            <v>71.993417166005571</v>
-          </cell>
-          <cell r="R4">
-            <v>71.993417166005571</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5" t="str">
-            <v>West Texas Intermediate (WTI)</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F5">
-            <v>2020</v>
-          </cell>
-          <cell r="G5" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H5" t="str">
-            <v>bbl</v>
-          </cell>
-          <cell r="I5" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K5">
-            <v>80.510277023790977</v>
-          </cell>
-          <cell r="L5">
-            <v>80.510277023790977</v>
-          </cell>
-          <cell r="M5">
-            <v>101.23700842278313</v>
-          </cell>
-          <cell r="N5">
-            <v>56.593726379407435</v>
-          </cell>
-          <cell r="O5">
-            <v>70.058740276108168</v>
-          </cell>
-          <cell r="P5">
-            <v>73.593270880805719</v>
-          </cell>
-          <cell r="Q5">
-            <v>69.593636593805385</v>
-          </cell>
-          <cell r="R5">
-            <v>69.593636593805385</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>Western Canadian Select (WCS)</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F6">
-            <v>2020</v>
-          </cell>
-          <cell r="G6" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H6" t="str">
-            <v>bbl</v>
-          </cell>
-          <cell r="I6" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K6">
-            <v>52.152776124136977</v>
-          </cell>
-          <cell r="L6">
-            <v>52.152776124136977</v>
-          </cell>
-          <cell r="M6">
-            <v>83.589219181497086</v>
-          </cell>
-          <cell r="N6">
-            <v>40.725433300622093</v>
-          </cell>
-          <cell r="O6">
-            <v>56.47426734117483</v>
-          </cell>
-          <cell r="P6">
-            <v>61.594368019804797</v>
-          </cell>
-          <cell r="Q6">
-            <v>57.594733732804457</v>
-          </cell>
-          <cell r="R6">
-            <v>57.594733732804457</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>Canadian Light Sweet (CLS)</v>
-          </cell>
-          <cell r="E7" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F7">
-            <v>2020</v>
-          </cell>
-          <cell r="G7" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H7" t="str">
-            <v>bbl</v>
-          </cell>
-          <cell r="I7" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K7">
-            <v>63.12185516878214</v>
-          </cell>
-          <cell r="L7">
-            <v>63.12185516878214</v>
-          </cell>
-          <cell r="M7">
-            <v>83.643254053638174</v>
-          </cell>
-          <cell r="N7">
-            <v>66.803155547502755</v>
-          </cell>
-          <cell r="O7">
-            <v>82.48669449603068</v>
-          </cell>
-          <cell r="P7">
-            <v>92.55153740118719</v>
-          </cell>
-          <cell r="Q7">
-            <v>85.336197147438611</v>
-          </cell>
-          <cell r="R7">
-            <v>85.336197147438611</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>Henry Hub</v>
-          </cell>
-          <cell r="E8" t="str">
-            <v>Natural Gas</v>
-          </cell>
-          <cell r="F8">
-            <v>2020</v>
-          </cell>
-          <cell r="G8" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H8" t="str">
-            <v>MMBtu</v>
-          </cell>
-          <cell r="I8" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K8">
-            <v>12.09484683970792</v>
-          </cell>
-          <cell r="L8">
-            <v>12.09484683970792</v>
-          </cell>
-          <cell r="M8">
-            <v>5.4809784896361426</v>
-          </cell>
-          <cell r="N8">
-            <v>3.0581775298508642</v>
-          </cell>
-          <cell r="O8">
-            <v>4.0159752892476659</v>
-          </cell>
-          <cell r="P8">
-            <v>3.5996708583002786</v>
-          </cell>
-          <cell r="Q8">
-            <v>3.5996708583002786</v>
-          </cell>
-          <cell r="R8">
-            <v>3.7556565954932908</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9" t="str">
-            <v>Nova Inventory Transfer (NIT)</v>
-          </cell>
-          <cell r="E9" t="str">
-            <v>Natural Gas</v>
-          </cell>
-          <cell r="F9">
-            <v>2020</v>
-          </cell>
-          <cell r="G9" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H9" t="str">
-            <v>MMBtu</v>
-          </cell>
-          <cell r="I9" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K9">
-            <v>10.156284763586822</v>
-          </cell>
-          <cell r="L9">
-            <v>10.156284763586822</v>
-          </cell>
-          <cell r="M9">
-            <v>4.3529394956316887</v>
-          </cell>
-          <cell r="N9">
-            <v>2.4527921015320051</v>
-          </cell>
-          <cell r="O9">
-            <v>2.9909258420177003</v>
-          </cell>
-          <cell r="P9">
-            <v>2.5533665288209977</v>
-          </cell>
-          <cell r="Q9">
-            <v>2.8797366866402228</v>
-          </cell>
-          <cell r="R9">
-            <v>3.0453215461220355</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11" t="str">
-            <v>Brent</v>
-          </cell>
-          <cell r="E11" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F11">
-            <v>2020</v>
-          </cell>
-          <cell r="G11" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H11" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I11" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K11">
-            <v>14.311056498313594</v>
-          </cell>
-          <cell r="L11">
-            <v>14.311058874991911</v>
-          </cell>
-          <cell r="M11">
-            <v>18.694133190132003</v>
-          </cell>
-          <cell r="N11">
-            <v>11.21620037411093</v>
-          </cell>
-          <cell r="O11">
-            <v>13.423701887148971</v>
-          </cell>
-          <cell r="P11">
-            <v>14.010283766575347</v>
-          </cell>
-          <cell r="Q11">
-            <v>13.272900410439801</v>
-          </cell>
-          <cell r="R11">
-            <v>13.272900410439801</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12" t="str">
-            <v>West Texas Intermediate (WTI)</v>
-          </cell>
-          <cell r="E12" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F12">
-            <v>2020</v>
-          </cell>
-          <cell r="G12" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H12" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I12" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K12">
-            <v>14.843025717835181</v>
-          </cell>
-          <cell r="L12">
-            <v>14.843028182859156</v>
-          </cell>
-          <cell r="M12">
-            <v>18.664247274966481</v>
-          </cell>
-          <cell r="N12">
-            <v>10.433724621712123</v>
-          </cell>
-          <cell r="O12">
-            <v>12.916218165078719</v>
-          </cell>
-          <cell r="P12">
-            <v>13.56785375289402</v>
-          </cell>
-          <cell r="Q12">
-            <v>12.830470396758475</v>
-          </cell>
-          <cell r="R12">
-            <v>12.830470396758475</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13" t="str">
-            <v>Western Canadian Select (WCS)</v>
-          </cell>
-          <cell r="E13" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F13">
-            <v>2020</v>
-          </cell>
-          <cell r="G13" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H13" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I13" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K13">
-            <v>9.6149836503272237</v>
-          </cell>
-          <cell r="L13">
-            <v>9.6149852471152126</v>
-          </cell>
-          <cell r="M13">
-            <v>15.410667310609007</v>
-          </cell>
-          <cell r="N13">
-            <v>7.5082166053163277</v>
-          </cell>
-          <cell r="O13">
-            <v>10.411748124742546</v>
-          </cell>
-          <cell r="P13">
-            <v>11.35570368448739</v>
-          </cell>
-          <cell r="Q13">
-            <v>10.618320328351839</v>
-          </cell>
-          <cell r="R13">
-            <v>10.618320328351839</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14" t="str">
-            <v>Canadian Light Sweet (CLS)</v>
-          </cell>
-          <cell r="E14" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F14">
-            <v>2020</v>
-          </cell>
-          <cell r="G14" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H14" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I14" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K14">
-            <v>11.637263642141473</v>
-          </cell>
-          <cell r="L14">
-            <v>11.63726557477532</v>
-          </cell>
-          <cell r="M14">
-            <v>15.420629282330859</v>
-          </cell>
-          <cell r="N14">
-            <v>12.315953965838542</v>
-          </cell>
-          <cell r="O14">
-            <v>15.207469298306304</v>
-          </cell>
-          <cell r="P14">
-            <v>17.063050860976503</v>
-          </cell>
-          <cell r="Q14">
-            <v>15.732811286507976</v>
-          </cell>
-          <cell r="R14">
-            <v>15.732811286507976</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15" t="str">
-            <v>Henry Hub</v>
-          </cell>
-          <cell r="E15" t="str">
-            <v>Natural Gas</v>
-          </cell>
-          <cell r="F15">
-            <v>2020</v>
-          </cell>
-          <cell r="G15" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H15" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I15" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K15">
-            <v>14.280530770624067</v>
-          </cell>
-          <cell r="L15">
-            <v>14.280530770624067</v>
-          </cell>
-          <cell r="M15">
-            <v>6.4714570603250188</v>
-          </cell>
-          <cell r="N15">
-            <v>3.6108268997411312</v>
-          </cell>
-          <cell r="O15">
-            <v>4.7417102053647948</v>
-          </cell>
-          <cell r="P15">
-            <v>4.2501745691652983</v>
-          </cell>
-          <cell r="Q15">
-            <v>4.2501745691652983</v>
-          </cell>
-          <cell r="R15">
-            <v>4.4343488004957941</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16" t="str">
-            <v>Nova Inventory Transfer (NIT)</v>
-          </cell>
-          <cell r="E16" t="str">
-            <v>Natural Gas</v>
-          </cell>
-          <cell r="F16">
-            <v>2020</v>
-          </cell>
-          <cell r="G16" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H16" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I16" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K16">
-            <v>11.991647269600687</v>
-          </cell>
-          <cell r="L16">
-            <v>11.991647269600687</v>
-          </cell>
-          <cell r="M16">
-            <v>5.1395678865441754</v>
-          </cell>
-          <cell r="N16">
-            <v>2.8960410614606298</v>
-          </cell>
-          <cell r="O16">
-            <v>3.5314220250696389</v>
-          </cell>
-          <cell r="P16">
-            <v>3.0147904943945849</v>
-          </cell>
-          <cell r="Q16">
-            <v>3.4001396553322385</v>
-          </cell>
-          <cell r="R16">
-            <v>3.5956476855138422</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="D17" t="str">
-            <v>Production cost</v>
-          </cell>
-          <cell r="E17" t="str">
-            <v>Electricity</v>
-          </cell>
-          <cell r="F17">
-            <v>2020</v>
-          </cell>
-          <cell r="G17" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H17" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I17" t="str">
-            <v>pyCIMS</v>
-          </cell>
-          <cell r="K17">
-            <v>1</v>
-          </cell>
-          <cell r="L17">
-            <v>1</v>
-          </cell>
-          <cell r="M17">
-            <v>1</v>
-          </cell>
-          <cell r="N17">
-            <v>1</v>
-          </cell>
-          <cell r="O17">
-            <v>1</v>
-          </cell>
-          <cell r="P17">
-            <v>1</v>
-          </cell>
-          <cell r="Q17">
-            <v>1</v>
-          </cell>
-          <cell r="R17">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18" t="str">
-            <v>Production cost</v>
-          </cell>
-          <cell r="E18" t="str">
-            <v>Electricity</v>
-          </cell>
-          <cell r="F18">
-            <v>2020</v>
-          </cell>
-          <cell r="G18" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H18" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I18" t="str">
-            <v>pyCIMS</v>
-          </cell>
-          <cell r="K18">
-            <v>1</v>
-          </cell>
-          <cell r="L18">
-            <v>1</v>
-          </cell>
-          <cell r="M18">
-            <v>1</v>
-          </cell>
-          <cell r="N18">
-            <v>1</v>
-          </cell>
-          <cell r="O18">
-            <v>1</v>
-          </cell>
-          <cell r="P18">
-            <v>1</v>
-          </cell>
-          <cell r="Q18">
-            <v>1</v>
-          </cell>
-          <cell r="R18">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="D19" t="str">
-            <v>Production cost</v>
-          </cell>
-          <cell r="E19" t="str">
-            <v>Electricity</v>
-          </cell>
-          <cell r="F19">
-            <v>2020</v>
-          </cell>
-          <cell r="G19" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H19" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I19" t="str">
-            <v>pyCIMS</v>
-          </cell>
-          <cell r="K19">
-            <v>1</v>
-          </cell>
-          <cell r="L19">
-            <v>1</v>
-          </cell>
-          <cell r="M19">
-            <v>1</v>
-          </cell>
-          <cell r="N19">
-            <v>1</v>
-          </cell>
-          <cell r="O19">
-            <v>1</v>
-          </cell>
-          <cell r="P19">
-            <v>1</v>
-          </cell>
-          <cell r="Q19">
-            <v>1</v>
-          </cell>
-          <cell r="R19">
-            <v>1</v>
-          </cell>
-        </row>
         <row r="26">
           <cell r="B26" t="str">
             <v>CM</v>
@@ -2443,25 +1852,25 @@
             <v>25.947561036380627</v>
           </cell>
           <cell r="L59">
-            <v>25.947561036380627</v>
+            <v>24.082454818513263</v>
           </cell>
           <cell r="M59">
-            <v>24.887150647840976</v>
+            <v>22.123800324256099</v>
           </cell>
           <cell r="N59">
-            <v>17.826515795134856</v>
+            <v>18.640557035238167</v>
           </cell>
           <cell r="O59">
-            <v>15.870329435559558</v>
+            <v>16.238965353219228</v>
           </cell>
           <cell r="P59">
-            <v>15.930427844669392</v>
+            <v>16.158852134510823</v>
           </cell>
           <cell r="Q59">
-            <v>15.830628425995824</v>
+            <v>15.453025039305359</v>
           </cell>
           <cell r="R59">
-            <v>16.495007580135809</v>
+            <v>16.511991373441937</v>
           </cell>
         </row>
         <row r="60">
@@ -2487,25 +1896,25 @@
             <v>15.829446753962097</v>
           </cell>
           <cell r="L60">
-            <v>15.829446753962097</v>
+            <v>16.052894367923386</v>
           </cell>
           <cell r="M60">
-            <v>15.737222436815371</v>
+            <v>15.151255238929304</v>
           </cell>
           <cell r="N60">
-            <v>12.867190205762206</v>
+            <v>11.518888243449233</v>
           </cell>
           <cell r="O60">
-            <v>9.6324675600947867</v>
+            <v>9.6896547475243846</v>
           </cell>
           <cell r="P60">
-            <v>9.4753512936852431</v>
+            <v>9.6925131882311373</v>
           </cell>
           <cell r="Q60">
-            <v>9.1760686193184977</v>
+            <v>8.845251921786204</v>
           </cell>
           <cell r="R60">
-            <v>9.8596811444474053</v>
+            <v>9.873815676017422</v>
           </cell>
         </row>
         <row r="61">
@@ -2531,25 +1940,25 @@
             <v>25.352936391503111</v>
           </cell>
           <cell r="L61">
-            <v>25.352936391503111</v>
+            <v>26.522662456461035</v>
           </cell>
           <cell r="M61">
-            <v>27.689634148856342</v>
+            <v>31.038449098847046</v>
           </cell>
           <cell r="N61">
-            <v>29.093849222101198</v>
+            <v>32.001029928008876</v>
           </cell>
           <cell r="O61">
-            <v>31.487633146999165</v>
+            <v>32.546031019052727</v>
           </cell>
           <cell r="P61">
-            <v>34.301817041496228</v>
+            <v>34.410841058493453</v>
           </cell>
           <cell r="Q61">
-            <v>34.54282017955169</v>
+            <v>33.647257014155734</v>
           </cell>
           <cell r="R61">
-            <v>34.595803026122553</v>
+            <v>34.631282775169552</v>
           </cell>
         </row>
         <row r="62">
@@ -2572,28 +1981,28 @@
             <v>CER</v>
           </cell>
           <cell r="K62">
-            <v>28.821698675148614</v>
+            <v>28.821698675148621</v>
           </cell>
           <cell r="L62">
-            <v>28.821698675148614</v>
+            <v>29.672570660409356</v>
           </cell>
           <cell r="M62">
-            <v>32.232010511145539</v>
+            <v>34.467857420610393</v>
           </cell>
           <cell r="N62">
-            <v>32.499820131145491</v>
+            <v>35.990931599746311</v>
           </cell>
           <cell r="O62">
-            <v>35.794556796014355</v>
+            <v>36.360356984034745</v>
           </cell>
           <cell r="P62">
-            <v>37.99714314931159</v>
+            <v>38.294112800246062</v>
           </cell>
           <cell r="Q62">
-            <v>38.800303489547581</v>
+            <v>37.756074317223209</v>
           </cell>
           <cell r="R62">
-            <v>38.743747565625355</v>
+            <v>38.771995724690626</v>
           </cell>
         </row>
         <row r="63">
@@ -2619,25 +2028,25 @@
             <v>24.5949470651965</v>
           </cell>
           <cell r="L63">
-            <v>24.5949470651965</v>
+            <v>26.127847418708804</v>
           </cell>
           <cell r="M63">
-            <v>27.421405921883405</v>
+            <v>29.437413692012804</v>
           </cell>
           <cell r="N63">
-            <v>25.934654364731465</v>
+            <v>29.404340443423816</v>
           </cell>
           <cell r="O63">
-            <v>26.825004115732948</v>
+            <v>29.212549581374688</v>
           </cell>
           <cell r="P63">
-            <v>29.650974941978415</v>
+            <v>29.812363408308013</v>
           </cell>
           <cell r="Q63">
-            <v>29.946222047230179</v>
+            <v>28.948947068289257</v>
           </cell>
           <cell r="R63">
-            <v>29.522278414384466</v>
+            <v>29.538104440716495</v>
           </cell>
         </row>
         <row r="64">
@@ -2660,28 +2069,28 @@
             <v>CER</v>
           </cell>
           <cell r="K64">
-            <v>26.307387342454344</v>
+            <v>26.307387342454348</v>
           </cell>
           <cell r="L64">
-            <v>26.307387342454344</v>
+            <v>27.766443280093405</v>
           </cell>
           <cell r="M64">
-            <v>28.840593201474896</v>
+            <v>31.003100280678144</v>
           </cell>
           <cell r="N64">
-            <v>27.276875826064266</v>
+            <v>30.406033816373508</v>
           </cell>
           <cell r="O64">
-            <v>29.43452674811622</v>
+            <v>31.128780967186096</v>
           </cell>
           <cell r="P64">
-            <v>32.71925503433593</v>
+            <v>32.937172878731303</v>
           </cell>
           <cell r="Q64">
-            <v>33.552377882431614</v>
+            <v>32.524220656595496</v>
           </cell>
           <cell r="R64">
-            <v>33.670366769615548</v>
+            <v>33.709276316024145</v>
           </cell>
         </row>
         <row r="65">
@@ -2707,25 +2116,25 @@
             <v>26.344507779252858</v>
           </cell>
           <cell r="L65">
-            <v>26.344507779252858</v>
+            <v>27.56986192557012</v>
           </cell>
           <cell r="M65">
-            <v>28.66079671753722</v>
+            <v>31.477652174688881</v>
           </cell>
           <cell r="N65">
-            <v>27.129309103725475</v>
+            <v>31.129548327702423</v>
           </cell>
           <cell r="O65">
-            <v>30.003394948656542</v>
+            <v>31.604595908566075</v>
           </cell>
           <cell r="P65">
-            <v>33.298686456795714</v>
+            <v>33.513171851361435</v>
           </cell>
           <cell r="Q65">
-            <v>34.17612746030732</v>
+            <v>33.138314758003986</v>
           </cell>
           <cell r="R65">
-            <v>34.292264261912543</v>
+            <v>34.332092106523262</v>
           </cell>
         </row>
         <row r="66">
@@ -2748,28 +2157,28 @@
             <v>CER</v>
           </cell>
           <cell r="K66">
-            <v>25.387432386254929</v>
+            <v>25.387432386254925</v>
           </cell>
           <cell r="L66">
-            <v>25.387432386254929</v>
+            <v>26.883349051437371</v>
           </cell>
           <cell r="M66">
-            <v>29.577686542763686</v>
+            <v>32.688740851856387</v>
           </cell>
           <cell r="N66">
-            <v>31.881950069412305</v>
+            <v>35.126820256992829</v>
           </cell>
           <cell r="O66">
-            <v>36.529347650698789</v>
+            <v>37.596004649861577</v>
           </cell>
           <cell r="P66">
-            <v>39.921492835306061</v>
+            <v>40.143990454254137</v>
           </cell>
           <cell r="Q66">
-            <v>40.829454685768781</v>
+            <v>39.785755561521491</v>
           </cell>
           <cell r="R66">
-            <v>40.937633375638221</v>
+            <v>40.977136782004109</v>
           </cell>
         </row>
         <row r="67">
@@ -2795,25 +2204,25 @@
             <v>24.341341709732479</v>
           </cell>
           <cell r="L67">
-            <v>24.341341709732479</v>
+            <v>25.608914088164056</v>
           </cell>
           <cell r="M67">
-            <v>26.598700737563217</v>
+            <v>30.147227119507146</v>
           </cell>
           <cell r="N67">
-            <v>28.748131391948977</v>
+            <v>31.417303464431658</v>
           </cell>
           <cell r="O67">
-            <v>29.73149549270876</v>
+            <v>31.991540269243615</v>
           </cell>
           <cell r="P67">
-            <v>34.683168423414791</v>
+            <v>34.173846979010698</v>
           </cell>
           <cell r="Q67">
-            <v>35.366451719759873</v>
+            <v>34.386873761680057</v>
           </cell>
           <cell r="R67">
-            <v>35.490302822565823</v>
+            <v>35.530687615305929</v>
           </cell>
         </row>
         <row r="68">
@@ -2839,25 +2248,25 @@
             <v>26.855017023975996</v>
           </cell>
           <cell r="L68">
-            <v>26.855017023975996</v>
+            <v>27.741720305278296</v>
           </cell>
           <cell r="M68">
-            <v>28.133103536234639</v>
+            <v>31.296655389641742</v>
           </cell>
           <cell r="N68">
-            <v>28.705856361209662</v>
+            <v>31.620989819489086</v>
           </cell>
           <cell r="O68">
-            <v>32.513681097749313</v>
+            <v>33.352819771614143</v>
           </cell>
           <cell r="P68">
-            <v>35.881475069032149</v>
+            <v>36.106673182794509</v>
           </cell>
           <cell r="Q68">
-            <v>36.743086283046622</v>
+            <v>35.709285994218078</v>
           </cell>
           <cell r="R68">
-            <v>36.864692174359</v>
+            <v>36.904783740901053</v>
           </cell>
         </row>
         <row r="69">
@@ -2880,28 +2289,28 @@
             <v>CER</v>
           </cell>
           <cell r="K69">
-            <v>26.879404574793426</v>
+            <v>26.879404574793423</v>
           </cell>
           <cell r="L69">
-            <v>26.879404574793426</v>
+            <v>27.145353618411637</v>
           </cell>
           <cell r="M69">
-            <v>25.909958864715819</v>
+            <v>29.941504748651546</v>
           </cell>
           <cell r="N69">
-            <v>27.967360096094254</v>
+            <v>29.938469006721071</v>
           </cell>
           <cell r="O69">
-            <v>30.416483768849162</v>
+            <v>30.446114878912262</v>
           </cell>
           <cell r="P69">
-            <v>33.583389323916819</v>
+            <v>33.776949931833144</v>
           </cell>
           <cell r="Q69">
-            <v>34.544638594886109</v>
+            <v>33.495427569674227</v>
           </cell>
           <cell r="R69">
-            <v>34.672813783375474</v>
+            <v>34.71114062517907</v>
           </cell>
         </row>
         <row r="70">
@@ -2927,25 +2336,25 @@
             <v>23.198173232822104</v>
           </cell>
           <cell r="L70">
-            <v>23.198173232822104</v>
+            <v>24.092543767125726</v>
           </cell>
           <cell r="M70">
-            <v>24.718896640091597</v>
+            <v>27.839648713974647</v>
           </cell>
           <cell r="N70">
-            <v>23.996369211665066</v>
+            <v>27.287507076220503</v>
           </cell>
           <cell r="O70">
-            <v>26.939011680945764</v>
+            <v>27.534192990092386</v>
           </cell>
           <cell r="P70">
-            <v>29.965752802285824</v>
+            <v>30.153873334091639</v>
           </cell>
           <cell r="Q70">
-            <v>30.85448000320909</v>
+            <v>29.826992352450326</v>
           </cell>
           <cell r="R70">
-            <v>31.011696870591216</v>
+            <v>31.04955985616585</v>
           </cell>
         </row>
         <row r="71">
@@ -2971,25 +2380,25 @@
             <v>25.636882590893777</v>
           </cell>
           <cell r="L71">
-            <v>25.636882590893777</v>
+            <v>26.760729527467635</v>
           </cell>
           <cell r="M71">
-            <v>27.255906089563879</v>
+            <v>29.952456718235371</v>
           </cell>
           <cell r="N71">
-            <v>23.545195458641519</v>
+            <v>28.630363687444657</v>
           </cell>
           <cell r="O71">
-            <v>25.766393810994195</v>
+            <v>26.658181223055639</v>
           </cell>
           <cell r="P71">
-            <v>24.923909788586894</v>
+            <v>25.282679391135336</v>
           </cell>
           <cell r="Q71">
-            <v>21.199318537751218</v>
+            <v>21.441032701939832</v>
           </cell>
           <cell r="R71">
-            <v>22.498007082101257</v>
+            <v>22.515575017085553</v>
           </cell>
         </row>
         <row r="72">
@@ -3015,25 +2424,25 @@
             <v>28.829318793142669</v>
           </cell>
           <cell r="L72">
-            <v>28.829318793142669</v>
+            <v>30.646568829533003</v>
           </cell>
           <cell r="M72">
-            <v>32.767394814606583</v>
+            <v>35.654923421149014</v>
           </cell>
           <cell r="N72">
-            <v>30.894233250201932</v>
+            <v>34.600422536036874</v>
           </cell>
           <cell r="O72">
-            <v>30.516719255515376</v>
+            <v>31.677618157208776</v>
           </cell>
           <cell r="P72">
-            <v>29.517081182076385</v>
+            <v>29.847595212122155</v>
           </cell>
           <cell r="Q72">
-            <v>25.905917982978266</v>
+            <v>26.130704108390105</v>
           </cell>
           <cell r="R72">
-            <v>27.198723015538619</v>
+            <v>27.213741304127076</v>
           </cell>
         </row>
         <row r="73">
@@ -3056,28 +2465,28 @@
             <v>CER</v>
           </cell>
           <cell r="K73">
-            <v>26.726587733652558</v>
+            <v>26.726587733652547</v>
           </cell>
           <cell r="L73">
-            <v>26.726587733652558</v>
+            <v>28.685890374583696</v>
           </cell>
           <cell r="M73">
-            <v>30.162292165124871</v>
+            <v>33.640923182695936</v>
           </cell>
           <cell r="N73">
-            <v>29.47736314732904</v>
+            <v>33.100730235732058</v>
           </cell>
           <cell r="O73">
-            <v>26.615701212805178</v>
+            <v>28.691896847622324</v>
           </cell>
           <cell r="P73">
-            <v>25.621158527607747</v>
+            <v>25.952659094981435</v>
           </cell>
           <cell r="Q73">
-            <v>22.002206272110072</v>
+            <v>22.226452016545977</v>
           </cell>
           <cell r="R73">
-            <v>23.298984314096462</v>
+            <v>23.314718018702955</v>
           </cell>
         </row>
         <row r="74">
@@ -3100,28 +2509,28 @@
             <v>CER</v>
           </cell>
           <cell r="K74">
-            <v>26.726587733652558</v>
+            <v>26.726587733652547</v>
           </cell>
           <cell r="L74">
-            <v>26.726587733652558</v>
+            <v>28.685890374583696</v>
           </cell>
           <cell r="M74">
-            <v>30.162292165124871</v>
+            <v>33.640923182695936</v>
           </cell>
           <cell r="N74">
-            <v>29.47736314732904</v>
+            <v>33.100730235732058</v>
           </cell>
           <cell r="O74">
-            <v>26.615701212805178</v>
+            <v>28.691896847622324</v>
           </cell>
           <cell r="P74">
-            <v>25.621158527607747</v>
+            <v>25.952659094981435</v>
           </cell>
           <cell r="Q74">
-            <v>22.002206272110072</v>
+            <v>22.226452016545977</v>
           </cell>
           <cell r="R74">
-            <v>23.298984314096462</v>
+            <v>23.314718018702955</v>
           </cell>
         </row>
       </sheetData>
@@ -3143,614 +2552,6 @@
             <v>Source</v>
           </cell>
         </row>
-        <row r="4">
-          <cell r="E4" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F4" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G4">
-            <v>2020</v>
-          </cell>
-          <cell r="H4" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I4" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L4">
-            <v>0</v>
-          </cell>
-          <cell r="M4">
-            <v>0</v>
-          </cell>
-          <cell r="N4">
-            <v>0</v>
-          </cell>
-          <cell r="O4">
-            <v>0</v>
-          </cell>
-          <cell r="P4">
-            <v>30</v>
-          </cell>
-          <cell r="Q4">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R4">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="E5" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F5" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G5">
-            <v>2020</v>
-          </cell>
-          <cell r="H5" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I5" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L5">
-            <v>0</v>
-          </cell>
-          <cell r="M5">
-            <v>0</v>
-          </cell>
-          <cell r="N5">
-            <v>26.526018458051627</v>
-          </cell>
-          <cell r="O5">
-            <v>33.304393348006798</v>
-          </cell>
-          <cell r="P5">
-            <v>40</v>
-          </cell>
-          <cell r="Q5">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R5">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="E6" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F6" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G6">
-            <v>2020</v>
-          </cell>
-          <cell r="H6" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I6" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L6">
-            <v>0</v>
-          </cell>
-          <cell r="M6">
-            <v>0</v>
-          </cell>
-          <cell r="N6">
-            <v>0</v>
-          </cell>
-          <cell r="O6">
-            <v>0</v>
-          </cell>
-          <cell r="P6">
-            <v>30</v>
-          </cell>
-          <cell r="Q6">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R6">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="E7" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F7" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G7">
-            <v>2020</v>
-          </cell>
-          <cell r="H7" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I7" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L7">
-            <v>0</v>
-          </cell>
-          <cell r="M7">
-            <v>0</v>
-          </cell>
-          <cell r="N7">
-            <v>0</v>
-          </cell>
-          <cell r="O7">
-            <v>0</v>
-          </cell>
-          <cell r="P7">
-            <v>30</v>
-          </cell>
-          <cell r="Q7">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R7">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="E8" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F8" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G8">
-            <v>2020</v>
-          </cell>
-          <cell r="H8" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I8" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L8">
-            <v>0</v>
-          </cell>
-          <cell r="M8">
-            <v>0</v>
-          </cell>
-          <cell r="N8">
-            <v>0</v>
-          </cell>
-          <cell r="O8">
-            <v>0</v>
-          </cell>
-          <cell r="P8">
-            <v>30</v>
-          </cell>
-          <cell r="Q8">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R8">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F9" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G9">
-            <v>2020</v>
-          </cell>
-          <cell r="H9" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I9" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L9">
-            <v>0</v>
-          </cell>
-          <cell r="M9">
-            <v>0</v>
-          </cell>
-          <cell r="N9">
-            <v>0</v>
-          </cell>
-          <cell r="O9">
-            <v>0</v>
-          </cell>
-          <cell r="P9">
-            <v>30</v>
-          </cell>
-          <cell r="Q9">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R9">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F10" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G10">
-            <v>2020</v>
-          </cell>
-          <cell r="H10" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I10" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L10">
-            <v>0</v>
-          </cell>
-          <cell r="M10">
-            <v>0</v>
-          </cell>
-          <cell r="N10">
-            <v>0</v>
-          </cell>
-          <cell r="O10">
-            <v>18.87248956387052</v>
-          </cell>
-          <cell r="P10">
-            <v>22.15</v>
-          </cell>
-          <cell r="Q10">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R10">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F11" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G11">
-            <v>2020</v>
-          </cell>
-          <cell r="H11" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I11" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L11">
-            <v>0</v>
-          </cell>
-          <cell r="M11">
-            <v>0</v>
-          </cell>
-          <cell r="N11">
-            <v>0</v>
-          </cell>
-          <cell r="O11">
-            <v>0</v>
-          </cell>
-          <cell r="P11">
-            <v>30</v>
-          </cell>
-          <cell r="Q11">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R11">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F12" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G12">
-            <v>2020</v>
-          </cell>
-          <cell r="H12" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I12" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L12">
-            <v>0</v>
-          </cell>
-          <cell r="M12">
-            <v>0</v>
-          </cell>
-          <cell r="N12">
-            <v>0</v>
-          </cell>
-          <cell r="O12">
-            <v>0</v>
-          </cell>
-          <cell r="P12">
-            <v>30</v>
-          </cell>
-          <cell r="Q12">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R12">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F13" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G13">
-            <v>2020</v>
-          </cell>
-          <cell r="H13" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I13" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L13">
-            <v>0</v>
-          </cell>
-          <cell r="M13">
-            <v>0</v>
-          </cell>
-          <cell r="N13">
-            <v>0</v>
-          </cell>
-          <cell r="O13">
-            <v>0</v>
-          </cell>
-          <cell r="P13">
-            <v>30</v>
-          </cell>
-          <cell r="Q13">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R13">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F14" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G14">
-            <v>2020</v>
-          </cell>
-          <cell r="H14" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I14" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L14">
-            <v>0</v>
-          </cell>
-          <cell r="M14">
-            <v>0</v>
-          </cell>
-          <cell r="N14">
-            <v>0</v>
-          </cell>
-          <cell r="O14">
-            <v>0</v>
-          </cell>
-          <cell r="P14">
-            <v>30</v>
-          </cell>
-          <cell r="Q14">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R14">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="E15" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F15" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G15">
-            <v>2020</v>
-          </cell>
-          <cell r="H15" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I15" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L15">
-            <v>0</v>
-          </cell>
-          <cell r="M15">
-            <v>0</v>
-          </cell>
-          <cell r="N15">
-            <v>0</v>
-          </cell>
-          <cell r="O15">
-            <v>0</v>
-          </cell>
-          <cell r="P15">
-            <v>30</v>
-          </cell>
-          <cell r="Q15">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R15">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F16" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G16">
-            <v>2020</v>
-          </cell>
-          <cell r="H16" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I16" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L16">
-            <v>0</v>
-          </cell>
-          <cell r="M16">
-            <v>0</v>
-          </cell>
-          <cell r="N16">
-            <v>0</v>
-          </cell>
-          <cell r="O16">
-            <v>0</v>
-          </cell>
-          <cell r="P16">
-            <v>30</v>
-          </cell>
-          <cell r="Q16">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R16">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F17" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G17">
-            <v>2020</v>
-          </cell>
-          <cell r="H17" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I17" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L17">
-            <v>0</v>
-          </cell>
-          <cell r="M17">
-            <v>0</v>
-          </cell>
-          <cell r="N17">
-            <v>0</v>
-          </cell>
-          <cell r="O17">
-            <v>0</v>
-          </cell>
-          <cell r="P17">
-            <v>30</v>
-          </cell>
-          <cell r="Q17">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R17">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F18" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G18">
-            <v>2020</v>
-          </cell>
-          <cell r="H18" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I18" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L18">
-            <v>0</v>
-          </cell>
-          <cell r="M18">
-            <v>0</v>
-          </cell>
-          <cell r="N18">
-            <v>0</v>
-          </cell>
-          <cell r="O18">
-            <v>0</v>
-          </cell>
-          <cell r="P18">
-            <v>30</v>
-          </cell>
-          <cell r="Q18">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R18">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F19" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G19">
-            <v>2020</v>
-          </cell>
-          <cell r="H19" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I19" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L19">
-            <v>0</v>
-          </cell>
-          <cell r="M19">
-            <v>0</v>
-          </cell>
-          <cell r="N19">
-            <v>0</v>
-          </cell>
-          <cell r="O19">
-            <v>0</v>
-          </cell>
-          <cell r="P19">
-            <v>30</v>
-          </cell>
-          <cell r="Q19">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R19">
-            <v>100.32134973994671</v>
-          </cell>
-        </row>
         <row r="24">
           <cell r="B24" t="str">
             <v>Need to check on process, CH4, N2O!!!</v>
@@ -4410,49 +3211,850 @@
       <sheetData sheetId="5">
         <row r="1">
           <cell r="D1" t="str">
-            <v>To</v>
-          </cell>
-          <cell r="G1" t="str">
-            <v>Multiply by</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4" t="str">
-            <v>Litre</v>
-          </cell>
-          <cell r="E4" t="str">
-            <v>l</v>
-          </cell>
-          <cell r="G4">
-            <v>3.7854000000000001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5" t="str">
-            <v>Gigajoule</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="G5">
-            <v>1.0550600000000001</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>Gigajoule</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="G6">
-            <v>3.6</v>
+            <v>Commercial</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Industrial</v>
+          </cell>
+          <cell r="G1">
+            <v>2000</v>
+          </cell>
+          <cell r="H1">
+            <v>2001</v>
+          </cell>
+          <cell r="I1">
+            <v>2002</v>
+          </cell>
+          <cell r="J1">
+            <v>2003</v>
+          </cell>
+          <cell r="K1">
+            <v>2004</v>
+          </cell>
+          <cell r="L1">
+            <v>2005</v>
+          </cell>
+          <cell r="M1">
+            <v>2006</v>
+          </cell>
+          <cell r="N1">
+            <v>2007</v>
+          </cell>
+          <cell r="O1">
+            <v>2008</v>
+          </cell>
+          <cell r="P1">
+            <v>2009</v>
+          </cell>
+          <cell r="Q1">
+            <v>2010</v>
+          </cell>
+          <cell r="R1">
+            <v>2011</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="D59">
+            <v>1.7</v>
+          </cell>
+          <cell r="E59">
+            <v>1.4</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="D60">
+            <v>1.4</v>
+          </cell>
+          <cell r="E60">
+            <v>1.05</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="D61">
+            <v>1.5</v>
+          </cell>
+          <cell r="E61">
+            <v>1.1000000000000001</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="D62">
+            <v>1.75</v>
+          </cell>
+          <cell r="E62">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="D63">
+            <v>1.85</v>
+          </cell>
+          <cell r="E63">
+            <v>1.25</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="D64">
+            <v>1.6</v>
+          </cell>
+          <cell r="E64">
+            <v>1.05</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="D65">
+            <v>1.6</v>
+          </cell>
+          <cell r="E65">
+            <v>1.2</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="D66">
+            <v>1.6</v>
+          </cell>
+          <cell r="E66">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="D67">
+            <v>1.4</v>
+          </cell>
+          <cell r="E67">
+            <v>1.2</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="D68">
+            <v>1.5</v>
+          </cell>
+          <cell r="E68">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="D69">
+            <v>1.5</v>
+          </cell>
+          <cell r="E69">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="D70">
+            <v>1.5</v>
+          </cell>
+          <cell r="E70">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="D71">
+            <v>1.6</v>
+          </cell>
+          <cell r="E71">
+            <v>1.125</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="D72">
+            <v>1.5</v>
+          </cell>
+          <cell r="E72">
+            <v>1.3</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="6">
         <row r="1">
           <cell r="D1" t="str">
+            <v>Sector</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Fuel</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>Unit</v>
+          </cell>
+          <cell r="I1" t="str">
+            <v>Source</v>
+          </cell>
+          <cell r="K1" t="str">
+            <v>Unit</v>
+          </cell>
+          <cell r="N1">
+            <v>1995</v>
+          </cell>
+          <cell r="O1">
+            <v>1996</v>
+          </cell>
+          <cell r="P1">
+            <v>1997</v>
+          </cell>
+          <cell r="Q1">
+            <v>1998</v>
+          </cell>
+          <cell r="R1">
+            <v>1999</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>CM</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>CNZ</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="D59" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E59" t="str">
+            <v>Natural Gas</v>
+          </cell>
+          <cell r="F59">
+            <v>2020</v>
+          </cell>
+          <cell r="G59" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H59" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I59" t="str">
+            <v>CER (avg calc)</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="D60" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E60" t="str">
+            <v>Natural Gas</v>
+          </cell>
+          <cell r="F60">
+            <v>2020</v>
+          </cell>
+          <cell r="G60" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H60" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I60" t="str">
+            <v>CER (avg calc)</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="D61" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E61" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F61">
+            <v>2020</v>
+          </cell>
+          <cell r="G61" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H61" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I61" t="str">
+            <v>CER (weighted avg calc)</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="D62" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E62" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F62">
+            <v>2020</v>
+          </cell>
+          <cell r="G62" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H62" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I62" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K62">
+            <v>2022</v>
+          </cell>
+          <cell r="L62" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M62" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N62">
+            <v>31.673392426239602</v>
+          </cell>
+          <cell r="O62">
+            <v>31.673392426239602</v>
+          </cell>
+          <cell r="P62">
+            <v>31.673392426239602</v>
+          </cell>
+          <cell r="Q62">
+            <v>31.673392426239602</v>
+          </cell>
+          <cell r="R62">
+            <v>31.673392426239602</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="D63" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E63" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F63">
+            <v>2020</v>
+          </cell>
+          <cell r="G63" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H63" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I63" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K63">
+            <v>2022</v>
+          </cell>
+          <cell r="L63" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M63" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N63">
+            <v>27.008549334206801</v>
+          </cell>
+          <cell r="O63">
+            <v>27.008549334206801</v>
+          </cell>
+          <cell r="P63">
+            <v>27.008549334206801</v>
+          </cell>
+          <cell r="Q63">
+            <v>27.008549334206801</v>
+          </cell>
+          <cell r="R63">
+            <v>27.008549334206801</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="D64" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E64" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F64">
+            <v>2020</v>
+          </cell>
+          <cell r="G64" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H64" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I64" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K64">
+            <v>2022</v>
+          </cell>
+          <cell r="L64" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M64" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N64">
+            <v>28.775457796757099</v>
+          </cell>
+          <cell r="O64">
+            <v>28.775457796757099</v>
+          </cell>
+          <cell r="P64">
+            <v>28.775457796757099</v>
+          </cell>
+          <cell r="Q64">
+            <v>28.775457796757099</v>
+          </cell>
+          <cell r="R64">
+            <v>28.775457796757099</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="D65" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E65" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F65">
+            <v>2020</v>
+          </cell>
+          <cell r="G65" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H65" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I65" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K65">
+            <v>2022</v>
+          </cell>
+          <cell r="L65" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M65" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N65">
+            <v>29.352571576593</v>
+          </cell>
+          <cell r="O65">
+            <v>29.352571576593</v>
+          </cell>
+          <cell r="P65">
+            <v>29.352571576593</v>
+          </cell>
+          <cell r="Q65">
+            <v>29.352571576593</v>
+          </cell>
+          <cell r="R65">
+            <v>29.352571576593</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="D66" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E66" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F66">
+            <v>2020</v>
+          </cell>
+          <cell r="G66" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H66" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I66" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K66">
+            <v>2022</v>
+          </cell>
+          <cell r="L66" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M66" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N66">
+            <v>28.047242860248399</v>
+          </cell>
+          <cell r="O66">
+            <v>28.047242860248399</v>
+          </cell>
+          <cell r="P66">
+            <v>28.047242860248399</v>
+          </cell>
+          <cell r="Q66">
+            <v>28.047242860248399</v>
+          </cell>
+          <cell r="R66">
+            <v>28.047242860248399</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="D67" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E67" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F67">
+            <v>2020</v>
+          </cell>
+          <cell r="G67" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H67" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I67" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K67">
+            <v>2022</v>
+          </cell>
+          <cell r="L67" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M67" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N67">
+            <v>26.9441056576105</v>
+          </cell>
+          <cell r="O67">
+            <v>26.9441056576105</v>
+          </cell>
+          <cell r="P67">
+            <v>26.9441056576105</v>
+          </cell>
+          <cell r="Q67">
+            <v>26.9441056576105</v>
+          </cell>
+          <cell r="R67">
+            <v>26.9441056576105</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="D68" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E68" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F68">
+            <v>2020</v>
+          </cell>
+          <cell r="G68" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H68" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I68" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K68">
+            <v>2022</v>
+          </cell>
+          <cell r="L68" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M68" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N68">
+            <v>29.902255412494501</v>
+          </cell>
+          <cell r="O68">
+            <v>29.902255412494501</v>
+          </cell>
+          <cell r="P68">
+            <v>29.902255412494501</v>
+          </cell>
+          <cell r="Q68">
+            <v>29.902255412494501</v>
+          </cell>
+          <cell r="R68">
+            <v>29.902255412494501</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="D69" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E69" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F69">
+            <v>2020</v>
+          </cell>
+          <cell r="G69" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H69" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I69" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K69">
+            <v>2022</v>
+          </cell>
+          <cell r="L69" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M69" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N69">
+            <v>30.076085031839199</v>
+          </cell>
+          <cell r="O69">
+            <v>30.076085031839199</v>
+          </cell>
+          <cell r="P69">
+            <v>30.076085031839199</v>
+          </cell>
+          <cell r="Q69">
+            <v>30.076085031839199</v>
+          </cell>
+          <cell r="R69">
+            <v>30.076085031839199</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="D70" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E70" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F70">
+            <v>2020</v>
+          </cell>
+          <cell r="G70" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H70" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I70" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K70">
+            <v>2022</v>
+          </cell>
+          <cell r="L70" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M70" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N70">
+            <v>26.545842901663001</v>
+          </cell>
+          <cell r="O70">
+            <v>26.545842901663001</v>
+          </cell>
+          <cell r="P70">
+            <v>26.545842901663001</v>
+          </cell>
+          <cell r="Q70">
+            <v>26.545842901663001</v>
+          </cell>
+          <cell r="R70">
+            <v>26.545842901663001</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="D71" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E71" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F71">
+            <v>2020</v>
+          </cell>
+          <cell r="G71" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H71" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I71" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K71">
+            <v>2022</v>
+          </cell>
+          <cell r="L71" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M71" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N71">
+            <v>28.2630102488435</v>
+          </cell>
+          <cell r="O71">
+            <v>28.2630102488435</v>
+          </cell>
+          <cell r="P71">
+            <v>28.2630102488435</v>
+          </cell>
+          <cell r="Q71">
+            <v>28.2630102488435</v>
+          </cell>
+          <cell r="R71">
+            <v>28.2630102488435</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="D72" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E72" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F72">
+            <v>2020</v>
+          </cell>
+          <cell r="G72" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H72" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I72" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K72">
+            <v>2022</v>
+          </cell>
+          <cell r="L72" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M72" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N72">
+            <v>31.7872712046324</v>
+          </cell>
+          <cell r="O72">
+            <v>31.7872712046324</v>
+          </cell>
+          <cell r="P72">
+            <v>31.7872712046324</v>
+          </cell>
+          <cell r="Q72">
+            <v>31.7872712046324</v>
+          </cell>
+          <cell r="R72">
+            <v>31.7872712046324</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="D73" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E73" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F73">
+            <v>2020</v>
+          </cell>
+          <cell r="G73" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H73" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I73" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K73">
+            <v>2022</v>
+          </cell>
+          <cell r="L73" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M73" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N73">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="O73">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="P73">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="Q73">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="R73">
+            <v>29.2279962328425</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="D74" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E74" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F74">
+            <v>2020</v>
+          </cell>
+          <cell r="G74" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H74" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I74" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K74">
+            <v>2022</v>
+          </cell>
+          <cell r="L74" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M74" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N74">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="O74">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="P74">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="Q74">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="R74">
+            <v>29.2279962328425</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7">
+        <row r="1">
+          <cell r="D1" t="str">
+            <v>To</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>Multiply by</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8">
+        <row r="1">
+          <cell r="D1" t="str">
             <v>For prices</v>
           </cell>
           <cell r="F1" t="str">
@@ -4493,666 +4095,11 @@
           </cell>
           <cell r="R1">
             <v>2011</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F5" t="str">
-            <v>AFDC</v>
-          </cell>
-          <cell r="G5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="H5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="I5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="J5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="K5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="L5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="M5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="N5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="O5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="P5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="Q5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="R5">
-            <v>33.322391017173047</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>Mm3</v>
-          </cell>
-          <cell r="G6">
-            <v>37.989999934966505</v>
-          </cell>
-          <cell r="H6">
-            <v>38.090000067537595</v>
-          </cell>
-          <cell r="I6">
-            <v>38.089999943885992</v>
-          </cell>
-          <cell r="J6">
-            <v>38.200000000000003</v>
-          </cell>
-          <cell r="K6">
-            <v>38.21000005608883</v>
-          </cell>
-          <cell r="L6">
-            <v>38.259998958056819</v>
-          </cell>
-          <cell r="M6">
-            <v>38.260000180720937</v>
-          </cell>
-          <cell r="N6">
-            <v>38.110000608339433</v>
-          </cell>
-          <cell r="O6">
-            <v>38.409998944225379</v>
-          </cell>
-          <cell r="P6">
-            <v>38.430000915151403</v>
-          </cell>
-          <cell r="Q6">
-            <v>38.51999993949601</v>
-          </cell>
-          <cell r="R6">
-            <v>38.560001088530569</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>kt</v>
-          </cell>
-          <cell r="F7" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G7">
-            <v>14</v>
-          </cell>
-          <cell r="H7">
-            <v>14</v>
-          </cell>
-          <cell r="I7">
-            <v>14</v>
-          </cell>
-          <cell r="J7">
-            <v>14</v>
-          </cell>
-          <cell r="K7">
-            <v>14</v>
-          </cell>
-          <cell r="L7">
-            <v>14.000000108315001</v>
-          </cell>
-          <cell r="M7">
-            <v>13.999999806108626</v>
-          </cell>
-          <cell r="N7">
-            <v>13.999999748986674</v>
-          </cell>
-          <cell r="O7">
-            <v>14.000000379920184</v>
-          </cell>
-          <cell r="P7">
-            <v>14.000000293094232</v>
-          </cell>
-          <cell r="Q7">
-            <v>13.999999509048447</v>
-          </cell>
-          <cell r="R7">
-            <v>13.999999576064937</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>kt</v>
-          </cell>
-          <cell r="F8" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G8">
-            <v>27.281135001993739</v>
-          </cell>
-          <cell r="H8">
-            <v>27.326522347523987</v>
-          </cell>
-          <cell r="I8">
-            <v>27.26900553429919</v>
-          </cell>
-          <cell r="J8">
-            <v>26.649636115461792</v>
-          </cell>
-          <cell r="K8">
-            <v>26.436665511450485</v>
-          </cell>
-          <cell r="L8">
-            <v>26.065005050848569</v>
-          </cell>
-          <cell r="M8">
-            <v>25.961495108007071</v>
-          </cell>
-          <cell r="N8">
-            <v>25.531014474531759</v>
-          </cell>
-          <cell r="O8">
-            <v>25.843172868753484</v>
-          </cell>
-          <cell r="P8">
-            <v>26.793021648355463</v>
-          </cell>
-          <cell r="Q8">
-            <v>26.786318243881073</v>
-          </cell>
-          <cell r="R8">
-            <v>26.168637600813259</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9" t="str">
-            <v>kt</v>
-          </cell>
-          <cell r="F9" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G9">
-            <v>28.830000239717378</v>
-          </cell>
-          <cell r="H9">
-            <v>28.82999995511139</v>
-          </cell>
-          <cell r="I9">
-            <v>28.830000015450388</v>
-          </cell>
-          <cell r="J9">
-            <v>28.82999994686336</v>
-          </cell>
-          <cell r="K9">
-            <v>28.829999901213348</v>
-          </cell>
-          <cell r="L9">
-            <v>28.830000062087507</v>
-          </cell>
-          <cell r="M9">
-            <v>28.829996791359196</v>
-          </cell>
-          <cell r="N9">
-            <v>28.829996297848346</v>
-          </cell>
-          <cell r="O9">
-            <v>28.829998215308454</v>
-          </cell>
-          <cell r="P9">
-            <v>28.83000207582332</v>
-          </cell>
-          <cell r="Q9">
-            <v>28.829995050999777</v>
-          </cell>
-          <cell r="R9">
-            <v>28.829996754598554</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="D10" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F10" t="str">
-            <v>StatCan, RESD</v>
-          </cell>
-          <cell r="G10">
-            <v>38.679925435948505</v>
-          </cell>
-          <cell r="H10">
-            <v>38.680065473475189</v>
-          </cell>
-          <cell r="I10">
-            <v>38.299955672007968</v>
-          </cell>
-          <cell r="J10">
-            <v>38.300019365322605</v>
-          </cell>
-          <cell r="K10">
-            <v>38.299998399923197</v>
-          </cell>
-          <cell r="L10">
-            <v>38.299931844114475</v>
-          </cell>
-          <cell r="M10">
-            <v>38.300002287300146</v>
-          </cell>
-          <cell r="N10">
-            <v>38.300022546602378</v>
-          </cell>
-          <cell r="O10">
-            <v>38.299933175988855</v>
-          </cell>
-          <cell r="P10">
-            <v>38.299956398350787</v>
-          </cell>
-          <cell r="Q10">
-            <v>38.299949311917906</v>
-          </cell>
-          <cell r="R10">
-            <v>38.300029726613161</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11" t="str">
-            <v>GWh</v>
-          </cell>
-          <cell r="F11" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G11">
-            <v>3.6</v>
-          </cell>
-          <cell r="H11">
-            <v>3.6</v>
-          </cell>
-          <cell r="I11">
-            <v>3.6</v>
-          </cell>
-          <cell r="J11">
-            <v>3.6</v>
-          </cell>
-          <cell r="K11">
-            <v>3.6</v>
-          </cell>
-          <cell r="L11">
-            <v>3.6</v>
-          </cell>
-          <cell r="M11">
-            <v>3.6</v>
-          </cell>
-          <cell r="N11">
-            <v>3.6</v>
-          </cell>
-          <cell r="O11">
-            <v>3.6</v>
-          </cell>
-          <cell r="P11">
-            <v>3.6</v>
-          </cell>
-          <cell r="Q11">
-            <v>3.6</v>
-          </cell>
-          <cell r="R11">
-            <v>3.6</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F12" t="str">
-            <v>AFDC</v>
-          </cell>
-          <cell r="G12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="H12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="I12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="J12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="K12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="L12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="M12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="N12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="O12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="P12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="Q12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="R12">
-            <v>21.275601056803168</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F13" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G13">
-            <v>42.500001679681141</v>
-          </cell>
-          <cell r="H13">
-            <v>42.500001372430312</v>
-          </cell>
-          <cell r="I13">
-            <v>42.500001853421082</v>
-          </cell>
-          <cell r="J13">
-            <v>42.500000153212326</v>
-          </cell>
-          <cell r="K13">
-            <v>42.500001555910806</v>
-          </cell>
-          <cell r="L13">
-            <v>42.49999462158479</v>
-          </cell>
-          <cell r="M13">
-            <v>42.499993198406727</v>
-          </cell>
-          <cell r="N13">
-            <v>42.500007934339692</v>
-          </cell>
-          <cell r="O13">
-            <v>42.500003902539106</v>
-          </cell>
-          <cell r="P13">
-            <v>42.500005927963386</v>
-          </cell>
-          <cell r="Q13">
-            <v>42.499996053265136</v>
-          </cell>
-          <cell r="R13">
-            <v>42.500008082757489</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F14" t="str">
-            <v>StatCan, RESD</v>
-          </cell>
-          <cell r="G14">
-            <v>34.659999168511533</v>
-          </cell>
-          <cell r="H14">
-            <v>34.659952530630569</v>
-          </cell>
-          <cell r="I14">
-            <v>34.99994930856888</v>
-          </cell>
-          <cell r="J14">
-            <v>35.000024944125158</v>
-          </cell>
-          <cell r="K14">
-            <v>35</v>
-          </cell>
-          <cell r="L14">
-            <v>34.999987755571823</v>
-          </cell>
-          <cell r="M14">
-            <v>35</v>
-          </cell>
-          <cell r="N14">
-            <v>35</v>
-          </cell>
-          <cell r="O14">
-            <v>35.000011988021569</v>
-          </cell>
-          <cell r="P14">
-            <v>34.999976328671664</v>
-          </cell>
-          <cell r="Q14">
-            <v>35.000023044660551</v>
-          </cell>
-          <cell r="R14">
-            <v>35</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15" t="str">
-            <v>kt</v>
-          </cell>
-          <cell r="F15" t="str">
-            <v>-</v>
-          </cell>
-          <cell r="G15">
-            <v>120</v>
-          </cell>
-          <cell r="H15">
-            <v>120</v>
-          </cell>
-          <cell r="I15">
-            <v>120</v>
-          </cell>
-          <cell r="J15">
-            <v>120</v>
-          </cell>
-          <cell r="K15">
-            <v>120</v>
-          </cell>
-          <cell r="L15">
-            <v>120</v>
-          </cell>
-          <cell r="M15">
-            <v>120</v>
-          </cell>
-          <cell r="N15">
-            <v>120</v>
-          </cell>
-          <cell r="O15">
-            <v>120</v>
-          </cell>
-          <cell r="P15">
-            <v>120</v>
-          </cell>
-          <cell r="Q15">
-            <v>120</v>
-          </cell>
-          <cell r="R15">
-            <v>120</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F16" t="str">
-            <v>StatCan, RESD</v>
-          </cell>
-          <cell r="G16">
-            <v>36.369907239712113</v>
-          </cell>
-          <cell r="H16">
-            <v>36.370010596962203</v>
-          </cell>
-          <cell r="I16">
-            <v>37.40004995420864</v>
-          </cell>
-          <cell r="J16">
-            <v>37.400067238191291</v>
-          </cell>
-          <cell r="K16">
-            <v>37.399981406303262</v>
-          </cell>
-          <cell r="L16">
-            <v>37.400184612679666</v>
-          </cell>
-          <cell r="M16">
-            <v>37.400059355987537</v>
-          </cell>
-          <cell r="N16">
-            <v>37.400157760962927</v>
-          </cell>
-          <cell r="O16">
-            <v>37.40004043482994</v>
-          </cell>
-          <cell r="P16">
-            <v>37.400068271036012</v>
-          </cell>
-          <cell r="Q16">
-            <v>37.400177462289264</v>
-          </cell>
-          <cell r="R16">
-            <v>37.400238829734306</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="D17" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F17" t="str">
-            <v>StatCan, RESD</v>
-          </cell>
-          <cell r="G17">
-            <v>26.84811029236986</v>
-          </cell>
-          <cell r="H17">
-            <v>26.84811029236986</v>
-          </cell>
-          <cell r="I17">
-            <v>26.84811029236986</v>
-          </cell>
-          <cell r="J17">
-            <v>26.800082610491533</v>
-          </cell>
-          <cell r="K17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="L17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="M17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="N17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="O17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="P17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="Q17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="R17">
-            <v>26.799897075220859</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18" t="str">
-            <v>Mm3</v>
-          </cell>
-          <cell r="F18" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G18">
-            <v>37.989999934966505</v>
-          </cell>
-          <cell r="H18">
-            <v>38.090000067537595</v>
-          </cell>
-          <cell r="I18">
-            <v>38.089999943885992</v>
-          </cell>
-          <cell r="J18">
-            <v>38.200000000000003</v>
-          </cell>
-          <cell r="K18">
-            <v>38.21000005608883</v>
-          </cell>
-          <cell r="L18">
-            <v>38.259998958056819</v>
-          </cell>
-          <cell r="M18">
-            <v>38.260000180720937</v>
-          </cell>
-          <cell r="N18">
-            <v>38.110000608339433</v>
-          </cell>
-          <cell r="O18">
-            <v>38.409998944225379</v>
-          </cell>
-          <cell r="P18">
-            <v>38.430000915151403</v>
-          </cell>
-          <cell r="Q18">
-            <v>38.51999993949601</v>
-          </cell>
-          <cell r="R18">
-            <v>38.560001088530569</v>
           </cell>
         </row>
         <row r="19">
           <cell r="B19" t="str">
             <v>Petroleum coke</v>
-          </cell>
-          <cell r="D19" t="str">
-            <v>kt</v>
-          </cell>
-          <cell r="F19" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G19">
-            <v>38.647544558124402</v>
-          </cell>
-          <cell r="H19">
-            <v>38.647544505439768</v>
-          </cell>
-          <cell r="I19">
-            <v>38.647544645524597</v>
-          </cell>
-          <cell r="J19">
-            <v>38.647544383625231</v>
-          </cell>
-          <cell r="K19">
-            <v>38.647544562117609</v>
-          </cell>
-          <cell r="L19">
-            <v>38.647544328371573</v>
-          </cell>
-          <cell r="M19">
-            <v>38.647538364410046</v>
-          </cell>
-          <cell r="N19">
-            <v>38.647532379989407</v>
-          </cell>
-          <cell r="O19">
-            <v>38.647536489743565</v>
-          </cell>
-          <cell r="P19">
-            <v>38.647537590620246</v>
-          </cell>
-          <cell r="Q19">
-            <v>38.647532447156081</v>
-          </cell>
-          <cell r="R19">
-            <v>38.647541819225708</v>
           </cell>
         </row>
         <row r="20">
@@ -6154,21 +5101,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1399EC-A8AD-491E-8CBF-A80BA9B0B353}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103DF7E6-4D3C-405A-9F8E-2718AFE29276}">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:X7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6242,7 +5189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -6298,7 +5245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -6315,7 +5262,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -6332,7 +5279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -6354,52 +5301,52 @@
       <c r="L6" t="s">
         <v>26</v>
       </c>
-      <c r="M6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(M$2,[1]!pyCIMS_year,0))</f>
+      <c r="M6" cm="1">
+        <f t="array" ref="M6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(M$2,[1]!CIMS_year))</f>
         <v>3004198</v>
       </c>
-      <c r="N6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(N$2,[1]!pyCIMS_year,0))</f>
+      <c r="N6" cm="1">
+        <f t="array" ref="N6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(N$2,[1]!CIMS_year))</f>
         <v>3321768</v>
       </c>
-      <c r="O6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(O$2,[1]!pyCIMS_year,0))</f>
+      <c r="O6" cm="1">
+        <f t="array" ref="O6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(O$2,[1]!CIMS_year))</f>
         <v>3732082</v>
       </c>
-      <c r="P6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(P$2,[1]!pyCIMS_year,0))</f>
+      <c r="P6" cm="1">
+        <f t="array" ref="P6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(P$2,[1]!CIMS_year))</f>
         <v>4144491</v>
       </c>
-      <c r="Q6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(Q$2,[1]!pyCIMS_year,0))</f>
+      <c r="Q6" cm="1">
+        <f t="array" ref="Q6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(Q$2,[1]!CIMS_year))</f>
         <v>4420029</v>
       </c>
-      <c r="R6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(R$2,[1]!pyCIMS_year,0))</f>
+      <c r="R6" cm="1">
+        <f t="array" ref="R6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(R$2,[1]!CIMS_year))</f>
         <v>4965000</v>
       </c>
-      <c r="S6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(S$2,[1]!pyCIMS_year,0))</f>
+      <c r="S6" cm="1">
+        <f t="array" ref="S6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(S$2,[1]!CIMS_year))</f>
         <v>5460100</v>
       </c>
-      <c r="T6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(T$2,[1]!pyCIMS_year,0))</f>
+      <c r="T6" cm="1">
+        <f t="array" ref="T6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(T$2,[1]!CIMS_year))</f>
         <v>5976700</v>
       </c>
-      <c r="U6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(U$2,[1]!pyCIMS_year,0))</f>
+      <c r="U6" cm="1">
+        <f t="array" ref="U6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(U$2,[1]!CIMS_year))</f>
         <v>6515600</v>
       </c>
-      <c r="V6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(V$2,[1]!pyCIMS_year,0))</f>
+      <c r="V6" cm="1">
+        <f t="array" ref="V6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(V$2,[1]!CIMS_year))</f>
         <v>6751778.2937559607</v>
       </c>
-      <c r="W6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(W$2,[1]!pyCIMS_year,0))</f>
+      <c r="W6" cm="1">
+        <f t="array" ref="W6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(W$2,[1]!CIMS_year))</f>
         <v>6981842.726861191</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -6421,48 +5368,48 @@
       <c r="L7" t="s">
         <v>28</v>
       </c>
-      <c r="M7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(M$2,[1]!pyCIMS_year,0))</f>
+      <c r="M7" cm="1">
+        <f t="array" ref="M7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(M$2,[1]!CIMS_year))</f>
         <v>241251.75158053398</v>
       </c>
-      <c r="N7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(N$2,[1]!pyCIMS_year,0))</f>
+      <c r="N7" cm="1">
+        <f t="array" ref="N7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(N$2,[1]!CIMS_year))</f>
         <v>286047.23224697507</v>
       </c>
-      <c r="O7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(O$2,[1]!pyCIMS_year,0))</f>
+      <c r="O7" cm="1">
+        <f t="array" ref="O7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(O$2,[1]!CIMS_year))</f>
         <v>311884.83832539228</v>
       </c>
-      <c r="P7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(P$2,[1]!pyCIMS_year,0))</f>
+      <c r="P7" cm="1">
+        <f t="array" ref="P7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(P$2,[1]!CIMS_year))</f>
         <v>371864.0496689151</v>
       </c>
-      <c r="Q7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(Q$2,[1]!pyCIMS_year,0))</f>
+      <c r="Q7" cm="1">
+        <f t="array" ref="Q7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(Q$2,[1]!CIMS_year))</f>
         <v>352708.69722059922</v>
       </c>
-      <c r="R7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(R$2,[1]!pyCIMS_year,0))</f>
+      <c r="R7" cm="1">
+        <f t="array" ref="R7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(R$2,[1]!CIMS_year))</f>
         <v>398094.70776005066</v>
       </c>
-      <c r="S7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(S$2,[1]!pyCIMS_year,0))</f>
+      <c r="S7" cm="1">
+        <f t="array" ref="S7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(S$2,[1]!CIMS_year))</f>
         <v>440960.56814001396</v>
       </c>
-      <c r="T7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(T$2,[1]!pyCIMS_year,0))</f>
+      <c r="T7" cm="1">
+        <f t="array" ref="T7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(T$2,[1]!CIMS_year))</f>
         <v>484955.42138564883</v>
       </c>
-      <c r="U7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(U$2,[1]!pyCIMS_year,0))</f>
+      <c r="U7" cm="1">
+        <f t="array" ref="U7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(U$2,[1]!CIMS_year))</f>
         <v>535701.75694266777</v>
       </c>
-      <c r="V7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(V$2,[1]!pyCIMS_year,0))</f>
+      <c r="V7" cm="1">
+        <f t="array" ref="V7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(V$2,[1]!CIMS_year))</f>
         <v>591527.46226970514</v>
       </c>
-      <c r="W7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(W$2,[1]!pyCIMS_year,0))</f>
+      <c r="W7" cm="1">
+        <f t="array" ref="W7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(W$2,[1]!CIMS_year))</f>
         <v>650318.67160160968</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Model update 250618 (#17)
* major revision of model and source files, updates to csv editor and results viewer, added policies, renamed sector files, updated Reference.ipynb
* update natural gas
* update csv files and sources for upstream and industrial sectors, latest version of Reference and Net Zero notebooks, latest version CSV Editor and Results Viewer

---------

Co-authored-by: Brad Griffin <bradford_griffin@sfu.ca>
</commit_message>
<xml_diff>
--- a/csv/model/CIMS_base/formula_CIMS_base_AB.xlsx
+++ b/csv/model/CIMS_base/formula_CIMS_base_AB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\CIMS_base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CIMS\dev\cims-models\csv\model\CIMS_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFD03DC2-A2BB-4DFD-AA19-29BB9516E724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36543896-C053-4CF5-BDDB-A404AE512B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40980" yWindow="4095" windowWidth="17280" windowHeight="8880" xr2:uid="{D4FDFC50-15E1-4CA4-93A0-790CA34B4E5C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14724549-7B89-4625-AD24-6A4785BB65F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="191029" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,6 +36,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -192,13 +214,15 @@
       <sheetName val="Prices"/>
       <sheetName val="Carbon_tax"/>
       <sheetName val="Demand"/>
+      <sheetName val="Elec markups"/>
+      <sheetName val="CER"/>
       <sheetName val="Conversions"/>
       <sheetName val="Coefficients"/>
     </sheetNames>
     <definedNames>
-      <definedName name="pyCIMS_GDP" refersTo="='Macro'!$D$59:$R$74"/>
-      <definedName name="pyCIMS_population" refersTo="='Macro'!$D$4:$R$19"/>
-      <definedName name="pyCIMS_year" refersTo="='Macro'!$D$1:$R$1"/>
+      <definedName name="CIMS_GDP" refersTo="='Macro'!$D$59:$R$74"/>
+      <definedName name="CIMS_population" refersTo="='Macro'!$D$4:$R$19"/>
+      <definedName name="CIMS_year" refersTo="='Macro'!$D$1:$R$1"/>
       <definedName name="region_CIMS" refersTo="='Control'!$B$19:$B$34"/>
     </definedNames>
     <sheetDataSet>
@@ -299,6 +323,51 @@
             <v>TR</v>
           </cell>
         </row>
+        <row r="59">
+          <cell r="D59" t="str">
+            <v>Industrial</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="D60" t="str">
+            <v>Commercial</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="D61" t="str">
+            <v>Industrial</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="D64" t="str">
+            <v>CER fuels</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="D65" t="str">
+            <v>Electricity</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="D66" t="str">
+            <v>Natural Gas</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="D67" t="str">
+            <v>Fuel Oil</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="D68" t="str">
+            <v>Gasoline</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="D69" t="str">
+            <v>Diesel</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="1">
@@ -1750,666 +1819,6 @@
             <v>2035</v>
           </cell>
         </row>
-        <row r="4">
-          <cell r="D4" t="str">
-            <v>Brent</v>
-          </cell>
-          <cell r="E4" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F4">
-            <v>2020</v>
-          </cell>
-          <cell r="G4" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H4" t="str">
-            <v>bbl</v>
-          </cell>
-          <cell r="I4" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K4">
-            <v>77.624814851455724</v>
-          </cell>
-          <cell r="L4">
-            <v>77.624814851455724</v>
-          </cell>
-          <cell r="M4">
-            <v>101.39911303920623</v>
-          </cell>
-          <cell r="N4">
-            <v>60.837965156576949</v>
-          </cell>
-          <cell r="O4">
-            <v>72.811378070272852</v>
-          </cell>
-          <cell r="P4">
-            <v>75.993051453005904</v>
-          </cell>
-          <cell r="Q4">
-            <v>71.993417166005571</v>
-          </cell>
-          <cell r="R4">
-            <v>71.993417166005571</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5" t="str">
-            <v>West Texas Intermediate (WTI)</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F5">
-            <v>2020</v>
-          </cell>
-          <cell r="G5" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H5" t="str">
-            <v>bbl</v>
-          </cell>
-          <cell r="I5" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K5">
-            <v>80.510277023790977</v>
-          </cell>
-          <cell r="L5">
-            <v>80.510277023790977</v>
-          </cell>
-          <cell r="M5">
-            <v>101.23700842278313</v>
-          </cell>
-          <cell r="N5">
-            <v>56.593726379407435</v>
-          </cell>
-          <cell r="O5">
-            <v>70.058740276108168</v>
-          </cell>
-          <cell r="P5">
-            <v>73.593270880805719</v>
-          </cell>
-          <cell r="Q5">
-            <v>69.593636593805385</v>
-          </cell>
-          <cell r="R5">
-            <v>69.593636593805385</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>Western Canadian Select (WCS)</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F6">
-            <v>2020</v>
-          </cell>
-          <cell r="G6" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H6" t="str">
-            <v>bbl</v>
-          </cell>
-          <cell r="I6" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K6">
-            <v>52.152776124136977</v>
-          </cell>
-          <cell r="L6">
-            <v>52.152776124136977</v>
-          </cell>
-          <cell r="M6">
-            <v>83.589219181497086</v>
-          </cell>
-          <cell r="N6">
-            <v>40.725433300622093</v>
-          </cell>
-          <cell r="O6">
-            <v>56.47426734117483</v>
-          </cell>
-          <cell r="P6">
-            <v>61.594368019804797</v>
-          </cell>
-          <cell r="Q6">
-            <v>57.594733732804457</v>
-          </cell>
-          <cell r="R6">
-            <v>57.594733732804457</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>Canadian Light Sweet (CLS)</v>
-          </cell>
-          <cell r="E7" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F7">
-            <v>2020</v>
-          </cell>
-          <cell r="G7" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H7" t="str">
-            <v>bbl</v>
-          </cell>
-          <cell r="I7" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K7">
-            <v>63.12185516878214</v>
-          </cell>
-          <cell r="L7">
-            <v>63.12185516878214</v>
-          </cell>
-          <cell r="M7">
-            <v>83.643254053638174</v>
-          </cell>
-          <cell r="N7">
-            <v>66.803155547502755</v>
-          </cell>
-          <cell r="O7">
-            <v>82.48669449603068</v>
-          </cell>
-          <cell r="P7">
-            <v>92.55153740118719</v>
-          </cell>
-          <cell r="Q7">
-            <v>85.336197147438611</v>
-          </cell>
-          <cell r="R7">
-            <v>85.336197147438611</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>Henry Hub</v>
-          </cell>
-          <cell r="E8" t="str">
-            <v>Natural Gas</v>
-          </cell>
-          <cell r="F8">
-            <v>2020</v>
-          </cell>
-          <cell r="G8" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H8" t="str">
-            <v>MMBtu</v>
-          </cell>
-          <cell r="I8" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K8">
-            <v>12.09484683970792</v>
-          </cell>
-          <cell r="L8">
-            <v>12.09484683970792</v>
-          </cell>
-          <cell r="M8">
-            <v>5.4809784896361426</v>
-          </cell>
-          <cell r="N8">
-            <v>3.0581775298508642</v>
-          </cell>
-          <cell r="O8">
-            <v>4.0159752892476659</v>
-          </cell>
-          <cell r="P8">
-            <v>3.5996708583002786</v>
-          </cell>
-          <cell r="Q8">
-            <v>3.5996708583002786</v>
-          </cell>
-          <cell r="R8">
-            <v>3.7556565954932908</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9" t="str">
-            <v>Nova Inventory Transfer (NIT)</v>
-          </cell>
-          <cell r="E9" t="str">
-            <v>Natural Gas</v>
-          </cell>
-          <cell r="F9">
-            <v>2020</v>
-          </cell>
-          <cell r="G9" t="str">
-            <v>USD</v>
-          </cell>
-          <cell r="H9" t="str">
-            <v>MMBtu</v>
-          </cell>
-          <cell r="I9" t="str">
-            <v>CER</v>
-          </cell>
-          <cell r="K9">
-            <v>10.156284763586822</v>
-          </cell>
-          <cell r="L9">
-            <v>10.156284763586822</v>
-          </cell>
-          <cell r="M9">
-            <v>4.3529394956316887</v>
-          </cell>
-          <cell r="N9">
-            <v>2.4527921015320051</v>
-          </cell>
-          <cell r="O9">
-            <v>2.9909258420177003</v>
-          </cell>
-          <cell r="P9">
-            <v>2.5533665288209977</v>
-          </cell>
-          <cell r="Q9">
-            <v>2.8797366866402228</v>
-          </cell>
-          <cell r="R9">
-            <v>3.0453215461220355</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11" t="str">
-            <v>Brent</v>
-          </cell>
-          <cell r="E11" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F11">
-            <v>2020</v>
-          </cell>
-          <cell r="G11" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H11" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I11" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K11">
-            <v>14.311056498313594</v>
-          </cell>
-          <cell r="L11">
-            <v>14.311058874991911</v>
-          </cell>
-          <cell r="M11">
-            <v>18.694133190132003</v>
-          </cell>
-          <cell r="N11">
-            <v>11.21620037411093</v>
-          </cell>
-          <cell r="O11">
-            <v>13.423701887148971</v>
-          </cell>
-          <cell r="P11">
-            <v>14.010283766575347</v>
-          </cell>
-          <cell r="Q11">
-            <v>13.272900410439801</v>
-          </cell>
-          <cell r="R11">
-            <v>13.272900410439801</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12" t="str">
-            <v>West Texas Intermediate (WTI)</v>
-          </cell>
-          <cell r="E12" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F12">
-            <v>2020</v>
-          </cell>
-          <cell r="G12" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H12" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I12" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K12">
-            <v>14.843025717835181</v>
-          </cell>
-          <cell r="L12">
-            <v>14.843028182859156</v>
-          </cell>
-          <cell r="M12">
-            <v>18.664247274966481</v>
-          </cell>
-          <cell r="N12">
-            <v>10.433724621712123</v>
-          </cell>
-          <cell r="O12">
-            <v>12.916218165078719</v>
-          </cell>
-          <cell r="P12">
-            <v>13.56785375289402</v>
-          </cell>
-          <cell r="Q12">
-            <v>12.830470396758475</v>
-          </cell>
-          <cell r="R12">
-            <v>12.830470396758475</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13" t="str">
-            <v>Western Canadian Select (WCS)</v>
-          </cell>
-          <cell r="E13" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F13">
-            <v>2020</v>
-          </cell>
-          <cell r="G13" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H13" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I13" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K13">
-            <v>9.6149836503272237</v>
-          </cell>
-          <cell r="L13">
-            <v>9.6149852471152126</v>
-          </cell>
-          <cell r="M13">
-            <v>15.410667310609007</v>
-          </cell>
-          <cell r="N13">
-            <v>7.5082166053163277</v>
-          </cell>
-          <cell r="O13">
-            <v>10.411748124742546</v>
-          </cell>
-          <cell r="P13">
-            <v>11.35570368448739</v>
-          </cell>
-          <cell r="Q13">
-            <v>10.618320328351839</v>
-          </cell>
-          <cell r="R13">
-            <v>10.618320328351839</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14" t="str">
-            <v>Canadian Light Sweet (CLS)</v>
-          </cell>
-          <cell r="E14" t="str">
-            <v>Oil</v>
-          </cell>
-          <cell r="F14">
-            <v>2020</v>
-          </cell>
-          <cell r="G14" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H14" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I14" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K14">
-            <v>11.637263642141473</v>
-          </cell>
-          <cell r="L14">
-            <v>11.63726557477532</v>
-          </cell>
-          <cell r="M14">
-            <v>15.420629282330859</v>
-          </cell>
-          <cell r="N14">
-            <v>12.315953965838542</v>
-          </cell>
-          <cell r="O14">
-            <v>15.207469298306304</v>
-          </cell>
-          <cell r="P14">
-            <v>17.063050860976503</v>
-          </cell>
-          <cell r="Q14">
-            <v>15.732811286507976</v>
-          </cell>
-          <cell r="R14">
-            <v>15.732811286507976</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15" t="str">
-            <v>Henry Hub</v>
-          </cell>
-          <cell r="E15" t="str">
-            <v>Natural Gas</v>
-          </cell>
-          <cell r="F15">
-            <v>2020</v>
-          </cell>
-          <cell r="G15" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H15" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I15" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K15">
-            <v>14.280530770624067</v>
-          </cell>
-          <cell r="L15">
-            <v>14.280530770624067</v>
-          </cell>
-          <cell r="M15">
-            <v>6.4714570603250188</v>
-          </cell>
-          <cell r="N15">
-            <v>3.6108268997411312</v>
-          </cell>
-          <cell r="O15">
-            <v>4.7417102053647948</v>
-          </cell>
-          <cell r="P15">
-            <v>4.2501745691652983</v>
-          </cell>
-          <cell r="Q15">
-            <v>4.2501745691652983</v>
-          </cell>
-          <cell r="R15">
-            <v>4.4343488004957941</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16" t="str">
-            <v>Nova Inventory Transfer (NIT)</v>
-          </cell>
-          <cell r="E16" t="str">
-            <v>Natural Gas</v>
-          </cell>
-          <cell r="F16">
-            <v>2020</v>
-          </cell>
-          <cell r="G16" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H16" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I16" t="str">
-            <v>calc</v>
-          </cell>
-          <cell r="K16">
-            <v>11.991647269600687</v>
-          </cell>
-          <cell r="L16">
-            <v>11.991647269600687</v>
-          </cell>
-          <cell r="M16">
-            <v>5.1395678865441754</v>
-          </cell>
-          <cell r="N16">
-            <v>2.8960410614606298</v>
-          </cell>
-          <cell r="O16">
-            <v>3.5314220250696389</v>
-          </cell>
-          <cell r="P16">
-            <v>3.0147904943945849</v>
-          </cell>
-          <cell r="Q16">
-            <v>3.4001396553322385</v>
-          </cell>
-          <cell r="R16">
-            <v>3.5956476855138422</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="D17" t="str">
-            <v>Production cost</v>
-          </cell>
-          <cell r="E17" t="str">
-            <v>Electricity</v>
-          </cell>
-          <cell r="F17">
-            <v>2020</v>
-          </cell>
-          <cell r="G17" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H17" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I17" t="str">
-            <v>pyCIMS</v>
-          </cell>
-          <cell r="K17">
-            <v>1</v>
-          </cell>
-          <cell r="L17">
-            <v>1</v>
-          </cell>
-          <cell r="M17">
-            <v>1</v>
-          </cell>
-          <cell r="N17">
-            <v>1</v>
-          </cell>
-          <cell r="O17">
-            <v>1</v>
-          </cell>
-          <cell r="P17">
-            <v>1</v>
-          </cell>
-          <cell r="Q17">
-            <v>1</v>
-          </cell>
-          <cell r="R17">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18" t="str">
-            <v>Production cost</v>
-          </cell>
-          <cell r="E18" t="str">
-            <v>Electricity</v>
-          </cell>
-          <cell r="F18">
-            <v>2020</v>
-          </cell>
-          <cell r="G18" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H18" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I18" t="str">
-            <v>pyCIMS</v>
-          </cell>
-          <cell r="K18">
-            <v>1</v>
-          </cell>
-          <cell r="L18">
-            <v>1</v>
-          </cell>
-          <cell r="M18">
-            <v>1</v>
-          </cell>
-          <cell r="N18">
-            <v>1</v>
-          </cell>
-          <cell r="O18">
-            <v>1</v>
-          </cell>
-          <cell r="P18">
-            <v>1</v>
-          </cell>
-          <cell r="Q18">
-            <v>1</v>
-          </cell>
-          <cell r="R18">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="D19" t="str">
-            <v>Production cost</v>
-          </cell>
-          <cell r="E19" t="str">
-            <v>Electricity</v>
-          </cell>
-          <cell r="F19">
-            <v>2020</v>
-          </cell>
-          <cell r="G19" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="H19" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="I19" t="str">
-            <v>pyCIMS</v>
-          </cell>
-          <cell r="K19">
-            <v>1</v>
-          </cell>
-          <cell r="L19">
-            <v>1</v>
-          </cell>
-          <cell r="M19">
-            <v>1</v>
-          </cell>
-          <cell r="N19">
-            <v>1</v>
-          </cell>
-          <cell r="O19">
-            <v>1</v>
-          </cell>
-          <cell r="P19">
-            <v>1</v>
-          </cell>
-          <cell r="Q19">
-            <v>1</v>
-          </cell>
-          <cell r="R19">
-            <v>1</v>
-          </cell>
-        </row>
         <row r="26">
           <cell r="B26" t="str">
             <v>CM</v>
@@ -2443,25 +1852,25 @@
             <v>25.947561036380627</v>
           </cell>
           <cell r="L59">
-            <v>25.947561036380627</v>
+            <v>24.082454818513263</v>
           </cell>
           <cell r="M59">
-            <v>24.887150647840976</v>
+            <v>22.123800324256099</v>
           </cell>
           <cell r="N59">
-            <v>17.826515795134856</v>
+            <v>18.640557035238167</v>
           </cell>
           <cell r="O59">
-            <v>15.870329435559558</v>
+            <v>16.238965353219228</v>
           </cell>
           <cell r="P59">
-            <v>15.930427844669392</v>
+            <v>16.158852134510823</v>
           </cell>
           <cell r="Q59">
-            <v>15.830628425995824</v>
+            <v>15.453025039305359</v>
           </cell>
           <cell r="R59">
-            <v>16.495007580135809</v>
+            <v>16.511991373441937</v>
           </cell>
         </row>
         <row r="60">
@@ -2487,25 +1896,25 @@
             <v>15.829446753962097</v>
           </cell>
           <cell r="L60">
-            <v>15.829446753962097</v>
+            <v>16.052894367923386</v>
           </cell>
           <cell r="M60">
-            <v>15.737222436815371</v>
+            <v>15.151255238929304</v>
           </cell>
           <cell r="N60">
-            <v>12.867190205762206</v>
+            <v>11.518888243449233</v>
           </cell>
           <cell r="O60">
-            <v>9.6324675600947867</v>
+            <v>9.6896547475243846</v>
           </cell>
           <cell r="P60">
-            <v>9.4753512936852431</v>
+            <v>9.6925131882311373</v>
           </cell>
           <cell r="Q60">
-            <v>9.1760686193184977</v>
+            <v>8.845251921786204</v>
           </cell>
           <cell r="R60">
-            <v>9.8596811444474053</v>
+            <v>9.873815676017422</v>
           </cell>
         </row>
         <row r="61">
@@ -2531,25 +1940,25 @@
             <v>25.352936391503111</v>
           </cell>
           <cell r="L61">
-            <v>25.352936391503111</v>
+            <v>26.522662456461035</v>
           </cell>
           <cell r="M61">
-            <v>27.689634148856342</v>
+            <v>31.038449098847046</v>
           </cell>
           <cell r="N61">
-            <v>29.093849222101198</v>
+            <v>32.001029928008876</v>
           </cell>
           <cell r="O61">
-            <v>31.487633146999165</v>
+            <v>32.546031019052727</v>
           </cell>
           <cell r="P61">
-            <v>34.301817041496228</v>
+            <v>34.410841058493453</v>
           </cell>
           <cell r="Q61">
-            <v>34.54282017955169</v>
+            <v>33.647257014155734</v>
           </cell>
           <cell r="R61">
-            <v>34.595803026122553</v>
+            <v>34.631282775169552</v>
           </cell>
         </row>
         <row r="62">
@@ -2572,28 +1981,28 @@
             <v>CER</v>
           </cell>
           <cell r="K62">
-            <v>28.821698675148614</v>
+            <v>28.821698675148621</v>
           </cell>
           <cell r="L62">
-            <v>28.821698675148614</v>
+            <v>29.672570660409356</v>
           </cell>
           <cell r="M62">
-            <v>32.232010511145539</v>
+            <v>34.467857420610393</v>
           </cell>
           <cell r="N62">
-            <v>32.499820131145491</v>
+            <v>35.990931599746311</v>
           </cell>
           <cell r="O62">
-            <v>35.794556796014355</v>
+            <v>36.360356984034745</v>
           </cell>
           <cell r="P62">
-            <v>37.99714314931159</v>
+            <v>38.294112800246062</v>
           </cell>
           <cell r="Q62">
-            <v>38.800303489547581</v>
+            <v>37.756074317223209</v>
           </cell>
           <cell r="R62">
-            <v>38.743747565625355</v>
+            <v>38.771995724690626</v>
           </cell>
         </row>
         <row r="63">
@@ -2619,25 +2028,25 @@
             <v>24.5949470651965</v>
           </cell>
           <cell r="L63">
-            <v>24.5949470651965</v>
+            <v>26.127847418708804</v>
           </cell>
           <cell r="M63">
-            <v>27.421405921883405</v>
+            <v>29.437413692012804</v>
           </cell>
           <cell r="N63">
-            <v>25.934654364731465</v>
+            <v>29.404340443423816</v>
           </cell>
           <cell r="O63">
-            <v>26.825004115732948</v>
+            <v>29.212549581374688</v>
           </cell>
           <cell r="P63">
-            <v>29.650974941978415</v>
+            <v>29.812363408308013</v>
           </cell>
           <cell r="Q63">
-            <v>29.946222047230179</v>
+            <v>28.948947068289257</v>
           </cell>
           <cell r="R63">
-            <v>29.522278414384466</v>
+            <v>29.538104440716495</v>
           </cell>
         </row>
         <row r="64">
@@ -2660,28 +2069,28 @@
             <v>CER</v>
           </cell>
           <cell r="K64">
-            <v>26.307387342454344</v>
+            <v>26.307387342454348</v>
           </cell>
           <cell r="L64">
-            <v>26.307387342454344</v>
+            <v>27.766443280093405</v>
           </cell>
           <cell r="M64">
-            <v>28.840593201474896</v>
+            <v>31.003100280678144</v>
           </cell>
           <cell r="N64">
-            <v>27.276875826064266</v>
+            <v>30.406033816373508</v>
           </cell>
           <cell r="O64">
-            <v>29.43452674811622</v>
+            <v>31.128780967186096</v>
           </cell>
           <cell r="P64">
-            <v>32.71925503433593</v>
+            <v>32.937172878731303</v>
           </cell>
           <cell r="Q64">
-            <v>33.552377882431614</v>
+            <v>32.524220656595496</v>
           </cell>
           <cell r="R64">
-            <v>33.670366769615548</v>
+            <v>33.709276316024145</v>
           </cell>
         </row>
         <row r="65">
@@ -2707,25 +2116,25 @@
             <v>26.344507779252858</v>
           </cell>
           <cell r="L65">
-            <v>26.344507779252858</v>
+            <v>27.56986192557012</v>
           </cell>
           <cell r="M65">
-            <v>28.66079671753722</v>
+            <v>31.477652174688881</v>
           </cell>
           <cell r="N65">
-            <v>27.129309103725475</v>
+            <v>31.129548327702423</v>
           </cell>
           <cell r="O65">
-            <v>30.003394948656542</v>
+            <v>31.604595908566075</v>
           </cell>
           <cell r="P65">
-            <v>33.298686456795714</v>
+            <v>33.513171851361435</v>
           </cell>
           <cell r="Q65">
-            <v>34.17612746030732</v>
+            <v>33.138314758003986</v>
           </cell>
           <cell r="R65">
-            <v>34.292264261912543</v>
+            <v>34.332092106523262</v>
           </cell>
         </row>
         <row r="66">
@@ -2748,28 +2157,28 @@
             <v>CER</v>
           </cell>
           <cell r="K66">
-            <v>25.387432386254929</v>
+            <v>25.387432386254925</v>
           </cell>
           <cell r="L66">
-            <v>25.387432386254929</v>
+            <v>26.883349051437371</v>
           </cell>
           <cell r="M66">
-            <v>29.577686542763686</v>
+            <v>32.688740851856387</v>
           </cell>
           <cell r="N66">
-            <v>31.881950069412305</v>
+            <v>35.126820256992829</v>
           </cell>
           <cell r="O66">
-            <v>36.529347650698789</v>
+            <v>37.596004649861577</v>
           </cell>
           <cell r="P66">
-            <v>39.921492835306061</v>
+            <v>40.143990454254137</v>
           </cell>
           <cell r="Q66">
-            <v>40.829454685768781</v>
+            <v>39.785755561521491</v>
           </cell>
           <cell r="R66">
-            <v>40.937633375638221</v>
+            <v>40.977136782004109</v>
           </cell>
         </row>
         <row r="67">
@@ -2795,25 +2204,25 @@
             <v>24.341341709732479</v>
           </cell>
           <cell r="L67">
-            <v>24.341341709732479</v>
+            <v>25.608914088164056</v>
           </cell>
           <cell r="M67">
-            <v>26.598700737563217</v>
+            <v>30.147227119507146</v>
           </cell>
           <cell r="N67">
-            <v>28.748131391948977</v>
+            <v>31.417303464431658</v>
           </cell>
           <cell r="O67">
-            <v>29.73149549270876</v>
+            <v>31.991540269243615</v>
           </cell>
           <cell r="P67">
-            <v>34.683168423414791</v>
+            <v>34.173846979010698</v>
           </cell>
           <cell r="Q67">
-            <v>35.366451719759873</v>
+            <v>34.386873761680057</v>
           </cell>
           <cell r="R67">
-            <v>35.490302822565823</v>
+            <v>35.530687615305929</v>
           </cell>
         </row>
         <row r="68">
@@ -2839,25 +2248,25 @@
             <v>26.855017023975996</v>
           </cell>
           <cell r="L68">
-            <v>26.855017023975996</v>
+            <v>27.741720305278296</v>
           </cell>
           <cell r="M68">
-            <v>28.133103536234639</v>
+            <v>31.296655389641742</v>
           </cell>
           <cell r="N68">
-            <v>28.705856361209662</v>
+            <v>31.620989819489086</v>
           </cell>
           <cell r="O68">
-            <v>32.513681097749313</v>
+            <v>33.352819771614143</v>
           </cell>
           <cell r="P68">
-            <v>35.881475069032149</v>
+            <v>36.106673182794509</v>
           </cell>
           <cell r="Q68">
-            <v>36.743086283046622</v>
+            <v>35.709285994218078</v>
           </cell>
           <cell r="R68">
-            <v>36.864692174359</v>
+            <v>36.904783740901053</v>
           </cell>
         </row>
         <row r="69">
@@ -2880,28 +2289,28 @@
             <v>CER</v>
           </cell>
           <cell r="K69">
-            <v>26.879404574793426</v>
+            <v>26.879404574793423</v>
           </cell>
           <cell r="L69">
-            <v>26.879404574793426</v>
+            <v>27.145353618411637</v>
           </cell>
           <cell r="M69">
-            <v>25.909958864715819</v>
+            <v>29.941504748651546</v>
           </cell>
           <cell r="N69">
-            <v>27.967360096094254</v>
+            <v>29.938469006721071</v>
           </cell>
           <cell r="O69">
-            <v>30.416483768849162</v>
+            <v>30.446114878912262</v>
           </cell>
           <cell r="P69">
-            <v>33.583389323916819</v>
+            <v>33.776949931833144</v>
           </cell>
           <cell r="Q69">
-            <v>34.544638594886109</v>
+            <v>33.495427569674227</v>
           </cell>
           <cell r="R69">
-            <v>34.672813783375474</v>
+            <v>34.71114062517907</v>
           </cell>
         </row>
         <row r="70">
@@ -2927,25 +2336,25 @@
             <v>23.198173232822104</v>
           </cell>
           <cell r="L70">
-            <v>23.198173232822104</v>
+            <v>24.092543767125726</v>
           </cell>
           <cell r="M70">
-            <v>24.718896640091597</v>
+            <v>27.839648713974647</v>
           </cell>
           <cell r="N70">
-            <v>23.996369211665066</v>
+            <v>27.287507076220503</v>
           </cell>
           <cell r="O70">
-            <v>26.939011680945764</v>
+            <v>27.534192990092386</v>
           </cell>
           <cell r="P70">
-            <v>29.965752802285824</v>
+            <v>30.153873334091639</v>
           </cell>
           <cell r="Q70">
-            <v>30.85448000320909</v>
+            <v>29.826992352450326</v>
           </cell>
           <cell r="R70">
-            <v>31.011696870591216</v>
+            <v>31.04955985616585</v>
           </cell>
         </row>
         <row r="71">
@@ -2971,25 +2380,25 @@
             <v>25.636882590893777</v>
           </cell>
           <cell r="L71">
-            <v>25.636882590893777</v>
+            <v>26.760729527467635</v>
           </cell>
           <cell r="M71">
-            <v>27.255906089563879</v>
+            <v>29.952456718235371</v>
           </cell>
           <cell r="N71">
-            <v>23.545195458641519</v>
+            <v>28.630363687444657</v>
           </cell>
           <cell r="O71">
-            <v>25.766393810994195</v>
+            <v>26.658181223055639</v>
           </cell>
           <cell r="P71">
-            <v>24.923909788586894</v>
+            <v>25.282679391135336</v>
           </cell>
           <cell r="Q71">
-            <v>21.199318537751218</v>
+            <v>21.441032701939832</v>
           </cell>
           <cell r="R71">
-            <v>22.498007082101257</v>
+            <v>22.515575017085553</v>
           </cell>
         </row>
         <row r="72">
@@ -3015,25 +2424,25 @@
             <v>28.829318793142669</v>
           </cell>
           <cell r="L72">
-            <v>28.829318793142669</v>
+            <v>30.646568829533003</v>
           </cell>
           <cell r="M72">
-            <v>32.767394814606583</v>
+            <v>35.654923421149014</v>
           </cell>
           <cell r="N72">
-            <v>30.894233250201932</v>
+            <v>34.600422536036874</v>
           </cell>
           <cell r="O72">
-            <v>30.516719255515376</v>
+            <v>31.677618157208776</v>
           </cell>
           <cell r="P72">
-            <v>29.517081182076385</v>
+            <v>29.847595212122155</v>
           </cell>
           <cell r="Q72">
-            <v>25.905917982978266</v>
+            <v>26.130704108390105</v>
           </cell>
           <cell r="R72">
-            <v>27.198723015538619</v>
+            <v>27.213741304127076</v>
           </cell>
         </row>
         <row r="73">
@@ -3056,28 +2465,28 @@
             <v>CER</v>
           </cell>
           <cell r="K73">
-            <v>26.726587733652558</v>
+            <v>26.726587733652547</v>
           </cell>
           <cell r="L73">
-            <v>26.726587733652558</v>
+            <v>28.685890374583696</v>
           </cell>
           <cell r="M73">
-            <v>30.162292165124871</v>
+            <v>33.640923182695936</v>
           </cell>
           <cell r="N73">
-            <v>29.47736314732904</v>
+            <v>33.100730235732058</v>
           </cell>
           <cell r="O73">
-            <v>26.615701212805178</v>
+            <v>28.691896847622324</v>
           </cell>
           <cell r="P73">
-            <v>25.621158527607747</v>
+            <v>25.952659094981435</v>
           </cell>
           <cell r="Q73">
-            <v>22.002206272110072</v>
+            <v>22.226452016545977</v>
           </cell>
           <cell r="R73">
-            <v>23.298984314096462</v>
+            <v>23.314718018702955</v>
           </cell>
         </row>
         <row r="74">
@@ -3100,28 +2509,28 @@
             <v>CER</v>
           </cell>
           <cell r="K74">
-            <v>26.726587733652558</v>
+            <v>26.726587733652547</v>
           </cell>
           <cell r="L74">
-            <v>26.726587733652558</v>
+            <v>28.685890374583696</v>
           </cell>
           <cell r="M74">
-            <v>30.162292165124871</v>
+            <v>33.640923182695936</v>
           </cell>
           <cell r="N74">
-            <v>29.47736314732904</v>
+            <v>33.100730235732058</v>
           </cell>
           <cell r="O74">
-            <v>26.615701212805178</v>
+            <v>28.691896847622324</v>
           </cell>
           <cell r="P74">
-            <v>25.621158527607747</v>
+            <v>25.952659094981435</v>
           </cell>
           <cell r="Q74">
-            <v>22.002206272110072</v>
+            <v>22.226452016545977</v>
           </cell>
           <cell r="R74">
-            <v>23.298984314096462</v>
+            <v>23.314718018702955</v>
           </cell>
         </row>
       </sheetData>
@@ -3143,614 +2552,6 @@
             <v>Source</v>
           </cell>
         </row>
-        <row r="4">
-          <cell r="E4" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F4" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G4">
-            <v>2020</v>
-          </cell>
-          <cell r="H4" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I4" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L4">
-            <v>0</v>
-          </cell>
-          <cell r="M4">
-            <v>0</v>
-          </cell>
-          <cell r="N4">
-            <v>0</v>
-          </cell>
-          <cell r="O4">
-            <v>0</v>
-          </cell>
-          <cell r="P4">
-            <v>30</v>
-          </cell>
-          <cell r="Q4">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R4">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="E5" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F5" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G5">
-            <v>2020</v>
-          </cell>
-          <cell r="H5" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I5" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L5">
-            <v>0</v>
-          </cell>
-          <cell r="M5">
-            <v>0</v>
-          </cell>
-          <cell r="N5">
-            <v>26.526018458051627</v>
-          </cell>
-          <cell r="O5">
-            <v>33.304393348006798</v>
-          </cell>
-          <cell r="P5">
-            <v>40</v>
-          </cell>
-          <cell r="Q5">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R5">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="E6" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F6" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G6">
-            <v>2020</v>
-          </cell>
-          <cell r="H6" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I6" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L6">
-            <v>0</v>
-          </cell>
-          <cell r="M6">
-            <v>0</v>
-          </cell>
-          <cell r="N6">
-            <v>0</v>
-          </cell>
-          <cell r="O6">
-            <v>0</v>
-          </cell>
-          <cell r="P6">
-            <v>30</v>
-          </cell>
-          <cell r="Q6">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R6">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="E7" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F7" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G7">
-            <v>2020</v>
-          </cell>
-          <cell r="H7" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I7" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L7">
-            <v>0</v>
-          </cell>
-          <cell r="M7">
-            <v>0</v>
-          </cell>
-          <cell r="N7">
-            <v>0</v>
-          </cell>
-          <cell r="O7">
-            <v>0</v>
-          </cell>
-          <cell r="P7">
-            <v>30</v>
-          </cell>
-          <cell r="Q7">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R7">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="E8" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F8" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G8">
-            <v>2020</v>
-          </cell>
-          <cell r="H8" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I8" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L8">
-            <v>0</v>
-          </cell>
-          <cell r="M8">
-            <v>0</v>
-          </cell>
-          <cell r="N8">
-            <v>0</v>
-          </cell>
-          <cell r="O8">
-            <v>0</v>
-          </cell>
-          <cell r="P8">
-            <v>30</v>
-          </cell>
-          <cell r="Q8">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R8">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F9" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G9">
-            <v>2020</v>
-          </cell>
-          <cell r="H9" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I9" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L9">
-            <v>0</v>
-          </cell>
-          <cell r="M9">
-            <v>0</v>
-          </cell>
-          <cell r="N9">
-            <v>0</v>
-          </cell>
-          <cell r="O9">
-            <v>0</v>
-          </cell>
-          <cell r="P9">
-            <v>30</v>
-          </cell>
-          <cell r="Q9">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R9">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F10" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G10">
-            <v>2020</v>
-          </cell>
-          <cell r="H10" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I10" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L10">
-            <v>0</v>
-          </cell>
-          <cell r="M10">
-            <v>0</v>
-          </cell>
-          <cell r="N10">
-            <v>0</v>
-          </cell>
-          <cell r="O10">
-            <v>18.87248956387052</v>
-          </cell>
-          <cell r="P10">
-            <v>22.15</v>
-          </cell>
-          <cell r="Q10">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R10">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F11" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G11">
-            <v>2020</v>
-          </cell>
-          <cell r="H11" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I11" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L11">
-            <v>0</v>
-          </cell>
-          <cell r="M11">
-            <v>0</v>
-          </cell>
-          <cell r="N11">
-            <v>0</v>
-          </cell>
-          <cell r="O11">
-            <v>0</v>
-          </cell>
-          <cell r="P11">
-            <v>30</v>
-          </cell>
-          <cell r="Q11">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R11">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F12" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G12">
-            <v>2020</v>
-          </cell>
-          <cell r="H12" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I12" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L12">
-            <v>0</v>
-          </cell>
-          <cell r="M12">
-            <v>0</v>
-          </cell>
-          <cell r="N12">
-            <v>0</v>
-          </cell>
-          <cell r="O12">
-            <v>0</v>
-          </cell>
-          <cell r="P12">
-            <v>30</v>
-          </cell>
-          <cell r="Q12">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R12">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F13" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G13">
-            <v>2020</v>
-          </cell>
-          <cell r="H13" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I13" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L13">
-            <v>0</v>
-          </cell>
-          <cell r="M13">
-            <v>0</v>
-          </cell>
-          <cell r="N13">
-            <v>0</v>
-          </cell>
-          <cell r="O13">
-            <v>0</v>
-          </cell>
-          <cell r="P13">
-            <v>30</v>
-          </cell>
-          <cell r="Q13">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R13">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F14" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G14">
-            <v>2020</v>
-          </cell>
-          <cell r="H14" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I14" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L14">
-            <v>0</v>
-          </cell>
-          <cell r="M14">
-            <v>0</v>
-          </cell>
-          <cell r="N14">
-            <v>0</v>
-          </cell>
-          <cell r="O14">
-            <v>0</v>
-          </cell>
-          <cell r="P14">
-            <v>30</v>
-          </cell>
-          <cell r="Q14">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R14">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="E15" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F15" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G15">
-            <v>2020</v>
-          </cell>
-          <cell r="H15" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I15" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L15">
-            <v>0</v>
-          </cell>
-          <cell r="M15">
-            <v>0</v>
-          </cell>
-          <cell r="N15">
-            <v>0</v>
-          </cell>
-          <cell r="O15">
-            <v>0</v>
-          </cell>
-          <cell r="P15">
-            <v>30</v>
-          </cell>
-          <cell r="Q15">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R15">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F16" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G16">
-            <v>2020</v>
-          </cell>
-          <cell r="H16" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I16" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L16">
-            <v>0</v>
-          </cell>
-          <cell r="M16">
-            <v>0</v>
-          </cell>
-          <cell r="N16">
-            <v>0</v>
-          </cell>
-          <cell r="O16">
-            <v>0</v>
-          </cell>
-          <cell r="P16">
-            <v>30</v>
-          </cell>
-          <cell r="Q16">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R16">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F17" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G17">
-            <v>2020</v>
-          </cell>
-          <cell r="H17" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I17" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L17">
-            <v>0</v>
-          </cell>
-          <cell r="M17">
-            <v>0</v>
-          </cell>
-          <cell r="N17">
-            <v>0</v>
-          </cell>
-          <cell r="O17">
-            <v>0</v>
-          </cell>
-          <cell r="P17">
-            <v>30</v>
-          </cell>
-          <cell r="Q17">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R17">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F18" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G18">
-            <v>2020</v>
-          </cell>
-          <cell r="H18" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I18" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L18">
-            <v>0</v>
-          </cell>
-          <cell r="M18">
-            <v>0</v>
-          </cell>
-          <cell r="N18">
-            <v>0</v>
-          </cell>
-          <cell r="O18">
-            <v>0</v>
-          </cell>
-          <cell r="P18">
-            <v>30</v>
-          </cell>
-          <cell r="Q18">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R18">
-            <v>100.32134973994673</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19" t="str">
-            <v>CO2</v>
-          </cell>
-          <cell r="F19" t="str">
-            <v>combustion</v>
-          </cell>
-          <cell r="G19">
-            <v>2020</v>
-          </cell>
-          <cell r="H19" t="str">
-            <v>CAD</v>
-          </cell>
-          <cell r="I19" t="str">
-            <v>tCO2</v>
-          </cell>
-          <cell r="L19">
-            <v>0</v>
-          </cell>
-          <cell r="M19">
-            <v>0</v>
-          </cell>
-          <cell r="N19">
-            <v>0</v>
-          </cell>
-          <cell r="O19">
-            <v>0</v>
-          </cell>
-          <cell r="P19">
-            <v>30</v>
-          </cell>
-          <cell r="Q19">
-            <v>68.341643330825832</v>
-          </cell>
-          <cell r="R19">
-            <v>100.32134973994671</v>
-          </cell>
-        </row>
         <row r="24">
           <cell r="B24" t="str">
             <v>Need to check on process, CH4, N2O!!!</v>
@@ -4410,49 +3211,850 @@
       <sheetData sheetId="5">
         <row r="1">
           <cell r="D1" t="str">
-            <v>To</v>
-          </cell>
-          <cell r="G1" t="str">
-            <v>Multiply by</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4" t="str">
-            <v>Litre</v>
-          </cell>
-          <cell r="E4" t="str">
-            <v>l</v>
-          </cell>
-          <cell r="G4">
-            <v>3.7854000000000001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5" t="str">
-            <v>Gigajoule</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="G5">
-            <v>1.0550600000000001</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>Gigajoule</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>GJ</v>
-          </cell>
-          <cell r="G6">
-            <v>3.6</v>
+            <v>Commercial</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Industrial</v>
+          </cell>
+          <cell r="G1">
+            <v>2000</v>
+          </cell>
+          <cell r="H1">
+            <v>2001</v>
+          </cell>
+          <cell r="I1">
+            <v>2002</v>
+          </cell>
+          <cell r="J1">
+            <v>2003</v>
+          </cell>
+          <cell r="K1">
+            <v>2004</v>
+          </cell>
+          <cell r="L1">
+            <v>2005</v>
+          </cell>
+          <cell r="M1">
+            <v>2006</v>
+          </cell>
+          <cell r="N1">
+            <v>2007</v>
+          </cell>
+          <cell r="O1">
+            <v>2008</v>
+          </cell>
+          <cell r="P1">
+            <v>2009</v>
+          </cell>
+          <cell r="Q1">
+            <v>2010</v>
+          </cell>
+          <cell r="R1">
+            <v>2011</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="D59">
+            <v>1.7</v>
+          </cell>
+          <cell r="E59">
+            <v>1.4</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="D60">
+            <v>1.4</v>
+          </cell>
+          <cell r="E60">
+            <v>1.05</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="D61">
+            <v>1.5</v>
+          </cell>
+          <cell r="E61">
+            <v>1.1000000000000001</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="D62">
+            <v>1.75</v>
+          </cell>
+          <cell r="E62">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="D63">
+            <v>1.85</v>
+          </cell>
+          <cell r="E63">
+            <v>1.25</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="D64">
+            <v>1.6</v>
+          </cell>
+          <cell r="E64">
+            <v>1.05</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="D65">
+            <v>1.6</v>
+          </cell>
+          <cell r="E65">
+            <v>1.2</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="D66">
+            <v>1.6</v>
+          </cell>
+          <cell r="E66">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="D67">
+            <v>1.4</v>
+          </cell>
+          <cell r="E67">
+            <v>1.2</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="D68">
+            <v>1.5</v>
+          </cell>
+          <cell r="E68">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="D69">
+            <v>1.5</v>
+          </cell>
+          <cell r="E69">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="D70">
+            <v>1.5</v>
+          </cell>
+          <cell r="E70">
+            <v>1.3</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="D71">
+            <v>1.6</v>
+          </cell>
+          <cell r="E71">
+            <v>1.125</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="D72">
+            <v>1.5</v>
+          </cell>
+          <cell r="E72">
+            <v>1.3</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="6">
         <row r="1">
           <cell r="D1" t="str">
+            <v>Sector</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Fuel</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>Unit</v>
+          </cell>
+          <cell r="I1" t="str">
+            <v>Source</v>
+          </cell>
+          <cell r="K1" t="str">
+            <v>Unit</v>
+          </cell>
+          <cell r="N1">
+            <v>1995</v>
+          </cell>
+          <cell r="O1">
+            <v>1996</v>
+          </cell>
+          <cell r="P1">
+            <v>1997</v>
+          </cell>
+          <cell r="Q1">
+            <v>1998</v>
+          </cell>
+          <cell r="R1">
+            <v>1999</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>CM</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>CNZ</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="D59" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E59" t="str">
+            <v>Natural Gas</v>
+          </cell>
+          <cell r="F59">
+            <v>2020</v>
+          </cell>
+          <cell r="G59" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H59" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I59" t="str">
+            <v>CER (avg calc)</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="D60" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E60" t="str">
+            <v>Natural Gas</v>
+          </cell>
+          <cell r="F60">
+            <v>2020</v>
+          </cell>
+          <cell r="G60" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H60" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I60" t="str">
+            <v>CER (avg calc)</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="D61" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E61" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F61">
+            <v>2020</v>
+          </cell>
+          <cell r="G61" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H61" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I61" t="str">
+            <v>CER (weighted avg calc)</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="D62" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E62" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F62">
+            <v>2020</v>
+          </cell>
+          <cell r="G62" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H62" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I62" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K62">
+            <v>2022</v>
+          </cell>
+          <cell r="L62" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M62" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N62">
+            <v>31.673392426239602</v>
+          </cell>
+          <cell r="O62">
+            <v>31.673392426239602</v>
+          </cell>
+          <cell r="P62">
+            <v>31.673392426239602</v>
+          </cell>
+          <cell r="Q62">
+            <v>31.673392426239602</v>
+          </cell>
+          <cell r="R62">
+            <v>31.673392426239602</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="D63" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E63" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F63">
+            <v>2020</v>
+          </cell>
+          <cell r="G63" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H63" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I63" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K63">
+            <v>2022</v>
+          </cell>
+          <cell r="L63" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M63" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N63">
+            <v>27.008549334206801</v>
+          </cell>
+          <cell r="O63">
+            <v>27.008549334206801</v>
+          </cell>
+          <cell r="P63">
+            <v>27.008549334206801</v>
+          </cell>
+          <cell r="Q63">
+            <v>27.008549334206801</v>
+          </cell>
+          <cell r="R63">
+            <v>27.008549334206801</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="D64" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E64" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F64">
+            <v>2020</v>
+          </cell>
+          <cell r="G64" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H64" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I64" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K64">
+            <v>2022</v>
+          </cell>
+          <cell r="L64" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M64" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N64">
+            <v>28.775457796757099</v>
+          </cell>
+          <cell r="O64">
+            <v>28.775457796757099</v>
+          </cell>
+          <cell r="P64">
+            <v>28.775457796757099</v>
+          </cell>
+          <cell r="Q64">
+            <v>28.775457796757099</v>
+          </cell>
+          <cell r="R64">
+            <v>28.775457796757099</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="D65" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E65" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F65">
+            <v>2020</v>
+          </cell>
+          <cell r="G65" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H65" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I65" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K65">
+            <v>2022</v>
+          </cell>
+          <cell r="L65" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M65" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N65">
+            <v>29.352571576593</v>
+          </cell>
+          <cell r="O65">
+            <v>29.352571576593</v>
+          </cell>
+          <cell r="P65">
+            <v>29.352571576593</v>
+          </cell>
+          <cell r="Q65">
+            <v>29.352571576593</v>
+          </cell>
+          <cell r="R65">
+            <v>29.352571576593</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="D66" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E66" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F66">
+            <v>2020</v>
+          </cell>
+          <cell r="G66" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H66" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I66" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K66">
+            <v>2022</v>
+          </cell>
+          <cell r="L66" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M66" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N66">
+            <v>28.047242860248399</v>
+          </cell>
+          <cell r="O66">
+            <v>28.047242860248399</v>
+          </cell>
+          <cell r="P66">
+            <v>28.047242860248399</v>
+          </cell>
+          <cell r="Q66">
+            <v>28.047242860248399</v>
+          </cell>
+          <cell r="R66">
+            <v>28.047242860248399</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="D67" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E67" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F67">
+            <v>2020</v>
+          </cell>
+          <cell r="G67" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H67" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I67" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K67">
+            <v>2022</v>
+          </cell>
+          <cell r="L67" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M67" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N67">
+            <v>26.9441056576105</v>
+          </cell>
+          <cell r="O67">
+            <v>26.9441056576105</v>
+          </cell>
+          <cell r="P67">
+            <v>26.9441056576105</v>
+          </cell>
+          <cell r="Q67">
+            <v>26.9441056576105</v>
+          </cell>
+          <cell r="R67">
+            <v>26.9441056576105</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="D68" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E68" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F68">
+            <v>2020</v>
+          </cell>
+          <cell r="G68" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H68" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I68" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K68">
+            <v>2022</v>
+          </cell>
+          <cell r="L68" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M68" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N68">
+            <v>29.902255412494501</v>
+          </cell>
+          <cell r="O68">
+            <v>29.902255412494501</v>
+          </cell>
+          <cell r="P68">
+            <v>29.902255412494501</v>
+          </cell>
+          <cell r="Q68">
+            <v>29.902255412494501</v>
+          </cell>
+          <cell r="R68">
+            <v>29.902255412494501</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="D69" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E69" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F69">
+            <v>2020</v>
+          </cell>
+          <cell r="G69" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H69" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I69" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K69">
+            <v>2022</v>
+          </cell>
+          <cell r="L69" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M69" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N69">
+            <v>30.076085031839199</v>
+          </cell>
+          <cell r="O69">
+            <v>30.076085031839199</v>
+          </cell>
+          <cell r="P69">
+            <v>30.076085031839199</v>
+          </cell>
+          <cell r="Q69">
+            <v>30.076085031839199</v>
+          </cell>
+          <cell r="R69">
+            <v>30.076085031839199</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="D70" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E70" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F70">
+            <v>2020</v>
+          </cell>
+          <cell r="G70" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H70" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I70" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K70">
+            <v>2022</v>
+          </cell>
+          <cell r="L70" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M70" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N70">
+            <v>26.545842901663001</v>
+          </cell>
+          <cell r="O70">
+            <v>26.545842901663001</v>
+          </cell>
+          <cell r="P70">
+            <v>26.545842901663001</v>
+          </cell>
+          <cell r="Q70">
+            <v>26.545842901663001</v>
+          </cell>
+          <cell r="R70">
+            <v>26.545842901663001</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="D71" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E71" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F71">
+            <v>2020</v>
+          </cell>
+          <cell r="G71" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H71" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I71" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K71">
+            <v>2022</v>
+          </cell>
+          <cell r="L71" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M71" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N71">
+            <v>28.2630102488435</v>
+          </cell>
+          <cell r="O71">
+            <v>28.2630102488435</v>
+          </cell>
+          <cell r="P71">
+            <v>28.2630102488435</v>
+          </cell>
+          <cell r="Q71">
+            <v>28.2630102488435</v>
+          </cell>
+          <cell r="R71">
+            <v>28.2630102488435</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="D72" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E72" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F72">
+            <v>2020</v>
+          </cell>
+          <cell r="G72" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H72" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I72" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K72">
+            <v>2022</v>
+          </cell>
+          <cell r="L72" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M72" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N72">
+            <v>31.7872712046324</v>
+          </cell>
+          <cell r="O72">
+            <v>31.7872712046324</v>
+          </cell>
+          <cell r="P72">
+            <v>31.7872712046324</v>
+          </cell>
+          <cell r="Q72">
+            <v>31.7872712046324</v>
+          </cell>
+          <cell r="R72">
+            <v>31.7872712046324</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="D73" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E73" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F73">
+            <v>2020</v>
+          </cell>
+          <cell r="G73" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H73" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I73" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K73">
+            <v>2022</v>
+          </cell>
+          <cell r="L73" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M73" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N73">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="O73">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="P73">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="Q73">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="R73">
+            <v>29.2279962328425</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="D74" t="str">
+            <v>Residential</v>
+          </cell>
+          <cell r="E74" t="str">
+            <v>Oil</v>
+          </cell>
+          <cell r="F74">
+            <v>2020</v>
+          </cell>
+          <cell r="G74" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="H74" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="I74" t="str">
+            <v>CER</v>
+          </cell>
+          <cell r="K74">
+            <v>2022</v>
+          </cell>
+          <cell r="L74" t="str">
+            <v>CAD</v>
+          </cell>
+          <cell r="M74" t="str">
+            <v>GJ</v>
+          </cell>
+          <cell r="N74">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="O74">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="P74">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="Q74">
+            <v>29.2279962328425</v>
+          </cell>
+          <cell r="R74">
+            <v>29.2279962328425</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7">
+        <row r="1">
+          <cell r="D1" t="str">
+            <v>To</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>Multiply by</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8">
+        <row r="1">
+          <cell r="D1" t="str">
             <v>For prices</v>
           </cell>
           <cell r="F1" t="str">
@@ -4493,666 +4095,11 @@
           </cell>
           <cell r="R1">
             <v>2011</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F5" t="str">
-            <v>AFDC</v>
-          </cell>
-          <cell r="G5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="H5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="I5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="J5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="K5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="L5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="M5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="N5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="O5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="P5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="Q5">
-            <v>33.322391017173047</v>
-          </cell>
-          <cell r="R5">
-            <v>33.322391017173047</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>Mm3</v>
-          </cell>
-          <cell r="G6">
-            <v>37.989999934966505</v>
-          </cell>
-          <cell r="H6">
-            <v>38.090000067537595</v>
-          </cell>
-          <cell r="I6">
-            <v>38.089999943885992</v>
-          </cell>
-          <cell r="J6">
-            <v>38.200000000000003</v>
-          </cell>
-          <cell r="K6">
-            <v>38.21000005608883</v>
-          </cell>
-          <cell r="L6">
-            <v>38.259998958056819</v>
-          </cell>
-          <cell r="M6">
-            <v>38.260000180720937</v>
-          </cell>
-          <cell r="N6">
-            <v>38.110000608339433</v>
-          </cell>
-          <cell r="O6">
-            <v>38.409998944225379</v>
-          </cell>
-          <cell r="P6">
-            <v>38.430000915151403</v>
-          </cell>
-          <cell r="Q6">
-            <v>38.51999993949601</v>
-          </cell>
-          <cell r="R6">
-            <v>38.560001088530569</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>kt</v>
-          </cell>
-          <cell r="F7" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G7">
-            <v>14</v>
-          </cell>
-          <cell r="H7">
-            <v>14</v>
-          </cell>
-          <cell r="I7">
-            <v>14</v>
-          </cell>
-          <cell r="J7">
-            <v>14</v>
-          </cell>
-          <cell r="K7">
-            <v>14</v>
-          </cell>
-          <cell r="L7">
-            <v>14.000000108315001</v>
-          </cell>
-          <cell r="M7">
-            <v>13.999999806108626</v>
-          </cell>
-          <cell r="N7">
-            <v>13.999999748986674</v>
-          </cell>
-          <cell r="O7">
-            <v>14.000000379920184</v>
-          </cell>
-          <cell r="P7">
-            <v>14.000000293094232</v>
-          </cell>
-          <cell r="Q7">
-            <v>13.999999509048447</v>
-          </cell>
-          <cell r="R7">
-            <v>13.999999576064937</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>kt</v>
-          </cell>
-          <cell r="F8" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G8">
-            <v>27.281135001993739</v>
-          </cell>
-          <cell r="H8">
-            <v>27.326522347523987</v>
-          </cell>
-          <cell r="I8">
-            <v>27.26900553429919</v>
-          </cell>
-          <cell r="J8">
-            <v>26.649636115461792</v>
-          </cell>
-          <cell r="K8">
-            <v>26.436665511450485</v>
-          </cell>
-          <cell r="L8">
-            <v>26.065005050848569</v>
-          </cell>
-          <cell r="M8">
-            <v>25.961495108007071</v>
-          </cell>
-          <cell r="N8">
-            <v>25.531014474531759</v>
-          </cell>
-          <cell r="O8">
-            <v>25.843172868753484</v>
-          </cell>
-          <cell r="P8">
-            <v>26.793021648355463</v>
-          </cell>
-          <cell r="Q8">
-            <v>26.786318243881073</v>
-          </cell>
-          <cell r="R8">
-            <v>26.168637600813259</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9" t="str">
-            <v>kt</v>
-          </cell>
-          <cell r="F9" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G9">
-            <v>28.830000239717378</v>
-          </cell>
-          <cell r="H9">
-            <v>28.82999995511139</v>
-          </cell>
-          <cell r="I9">
-            <v>28.830000015450388</v>
-          </cell>
-          <cell r="J9">
-            <v>28.82999994686336</v>
-          </cell>
-          <cell r="K9">
-            <v>28.829999901213348</v>
-          </cell>
-          <cell r="L9">
-            <v>28.830000062087507</v>
-          </cell>
-          <cell r="M9">
-            <v>28.829996791359196</v>
-          </cell>
-          <cell r="N9">
-            <v>28.829996297848346</v>
-          </cell>
-          <cell r="O9">
-            <v>28.829998215308454</v>
-          </cell>
-          <cell r="P9">
-            <v>28.83000207582332</v>
-          </cell>
-          <cell r="Q9">
-            <v>28.829995050999777</v>
-          </cell>
-          <cell r="R9">
-            <v>28.829996754598554</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="D10" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F10" t="str">
-            <v>StatCan, RESD</v>
-          </cell>
-          <cell r="G10">
-            <v>38.679925435948505</v>
-          </cell>
-          <cell r="H10">
-            <v>38.680065473475189</v>
-          </cell>
-          <cell r="I10">
-            <v>38.299955672007968</v>
-          </cell>
-          <cell r="J10">
-            <v>38.300019365322605</v>
-          </cell>
-          <cell r="K10">
-            <v>38.299998399923197</v>
-          </cell>
-          <cell r="L10">
-            <v>38.299931844114475</v>
-          </cell>
-          <cell r="M10">
-            <v>38.300002287300146</v>
-          </cell>
-          <cell r="N10">
-            <v>38.300022546602378</v>
-          </cell>
-          <cell r="O10">
-            <v>38.299933175988855</v>
-          </cell>
-          <cell r="P10">
-            <v>38.299956398350787</v>
-          </cell>
-          <cell r="Q10">
-            <v>38.299949311917906</v>
-          </cell>
-          <cell r="R10">
-            <v>38.300029726613161</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11" t="str">
-            <v>GWh</v>
-          </cell>
-          <cell r="F11" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G11">
-            <v>3.6</v>
-          </cell>
-          <cell r="H11">
-            <v>3.6</v>
-          </cell>
-          <cell r="I11">
-            <v>3.6</v>
-          </cell>
-          <cell r="J11">
-            <v>3.6</v>
-          </cell>
-          <cell r="K11">
-            <v>3.6</v>
-          </cell>
-          <cell r="L11">
-            <v>3.6</v>
-          </cell>
-          <cell r="M11">
-            <v>3.6</v>
-          </cell>
-          <cell r="N11">
-            <v>3.6</v>
-          </cell>
-          <cell r="O11">
-            <v>3.6</v>
-          </cell>
-          <cell r="P11">
-            <v>3.6</v>
-          </cell>
-          <cell r="Q11">
-            <v>3.6</v>
-          </cell>
-          <cell r="R11">
-            <v>3.6</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F12" t="str">
-            <v>AFDC</v>
-          </cell>
-          <cell r="G12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="H12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="I12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="J12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="K12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="L12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="M12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="N12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="O12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="P12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="Q12">
-            <v>21.275601056803168</v>
-          </cell>
-          <cell r="R12">
-            <v>21.275601056803168</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F13" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G13">
-            <v>42.500001679681141</v>
-          </cell>
-          <cell r="H13">
-            <v>42.500001372430312</v>
-          </cell>
-          <cell r="I13">
-            <v>42.500001853421082</v>
-          </cell>
-          <cell r="J13">
-            <v>42.500000153212326</v>
-          </cell>
-          <cell r="K13">
-            <v>42.500001555910806</v>
-          </cell>
-          <cell r="L13">
-            <v>42.49999462158479</v>
-          </cell>
-          <cell r="M13">
-            <v>42.499993198406727</v>
-          </cell>
-          <cell r="N13">
-            <v>42.500007934339692</v>
-          </cell>
-          <cell r="O13">
-            <v>42.500003902539106</v>
-          </cell>
-          <cell r="P13">
-            <v>42.500005927963386</v>
-          </cell>
-          <cell r="Q13">
-            <v>42.499996053265136</v>
-          </cell>
-          <cell r="R13">
-            <v>42.500008082757489</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F14" t="str">
-            <v>StatCan, RESD</v>
-          </cell>
-          <cell r="G14">
-            <v>34.659999168511533</v>
-          </cell>
-          <cell r="H14">
-            <v>34.659952530630569</v>
-          </cell>
-          <cell r="I14">
-            <v>34.99994930856888</v>
-          </cell>
-          <cell r="J14">
-            <v>35.000024944125158</v>
-          </cell>
-          <cell r="K14">
-            <v>35</v>
-          </cell>
-          <cell r="L14">
-            <v>34.999987755571823</v>
-          </cell>
-          <cell r="M14">
-            <v>35</v>
-          </cell>
-          <cell r="N14">
-            <v>35</v>
-          </cell>
-          <cell r="O14">
-            <v>35.000011988021569</v>
-          </cell>
-          <cell r="P14">
-            <v>34.999976328671664</v>
-          </cell>
-          <cell r="Q14">
-            <v>35.000023044660551</v>
-          </cell>
-          <cell r="R14">
-            <v>35</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15" t="str">
-            <v>kt</v>
-          </cell>
-          <cell r="F15" t="str">
-            <v>-</v>
-          </cell>
-          <cell r="G15">
-            <v>120</v>
-          </cell>
-          <cell r="H15">
-            <v>120</v>
-          </cell>
-          <cell r="I15">
-            <v>120</v>
-          </cell>
-          <cell r="J15">
-            <v>120</v>
-          </cell>
-          <cell r="K15">
-            <v>120</v>
-          </cell>
-          <cell r="L15">
-            <v>120</v>
-          </cell>
-          <cell r="M15">
-            <v>120</v>
-          </cell>
-          <cell r="N15">
-            <v>120</v>
-          </cell>
-          <cell r="O15">
-            <v>120</v>
-          </cell>
-          <cell r="P15">
-            <v>120</v>
-          </cell>
-          <cell r="Q15">
-            <v>120</v>
-          </cell>
-          <cell r="R15">
-            <v>120</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F16" t="str">
-            <v>StatCan, RESD</v>
-          </cell>
-          <cell r="G16">
-            <v>36.369907239712113</v>
-          </cell>
-          <cell r="H16">
-            <v>36.370010596962203</v>
-          </cell>
-          <cell r="I16">
-            <v>37.40004995420864</v>
-          </cell>
-          <cell r="J16">
-            <v>37.400067238191291</v>
-          </cell>
-          <cell r="K16">
-            <v>37.399981406303262</v>
-          </cell>
-          <cell r="L16">
-            <v>37.400184612679666</v>
-          </cell>
-          <cell r="M16">
-            <v>37.400059355987537</v>
-          </cell>
-          <cell r="N16">
-            <v>37.400157760962927</v>
-          </cell>
-          <cell r="O16">
-            <v>37.40004043482994</v>
-          </cell>
-          <cell r="P16">
-            <v>37.400068271036012</v>
-          </cell>
-          <cell r="Q16">
-            <v>37.400177462289264</v>
-          </cell>
-          <cell r="R16">
-            <v>37.400238829734306</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="D17" t="str">
-            <v>ML</v>
-          </cell>
-          <cell r="F17" t="str">
-            <v>StatCan, RESD</v>
-          </cell>
-          <cell r="G17">
-            <v>26.84811029236986</v>
-          </cell>
-          <cell r="H17">
-            <v>26.84811029236986</v>
-          </cell>
-          <cell r="I17">
-            <v>26.84811029236986</v>
-          </cell>
-          <cell r="J17">
-            <v>26.800082610491533</v>
-          </cell>
-          <cell r="K17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="L17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="M17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="N17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="O17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="P17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="Q17">
-            <v>26.799897075220859</v>
-          </cell>
-          <cell r="R17">
-            <v>26.799897075220859</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18" t="str">
-            <v>Mm3</v>
-          </cell>
-          <cell r="F18" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G18">
-            <v>37.989999934966505</v>
-          </cell>
-          <cell r="H18">
-            <v>38.090000067537595</v>
-          </cell>
-          <cell r="I18">
-            <v>38.089999943885992</v>
-          </cell>
-          <cell r="J18">
-            <v>38.200000000000003</v>
-          </cell>
-          <cell r="K18">
-            <v>38.21000005608883</v>
-          </cell>
-          <cell r="L18">
-            <v>38.259998958056819</v>
-          </cell>
-          <cell r="M18">
-            <v>38.260000180720937</v>
-          </cell>
-          <cell r="N18">
-            <v>38.110000608339433</v>
-          </cell>
-          <cell r="O18">
-            <v>38.409998944225379</v>
-          </cell>
-          <cell r="P18">
-            <v>38.430000915151403</v>
-          </cell>
-          <cell r="Q18">
-            <v>38.51999993949601</v>
-          </cell>
-          <cell r="R18">
-            <v>38.560001088530569</v>
           </cell>
         </row>
         <row r="19">
           <cell r="B19" t="str">
             <v>Petroleum coke</v>
-          </cell>
-          <cell r="D19" t="str">
-            <v>kt</v>
-          </cell>
-          <cell r="F19" t="str">
-            <v>StatCan, ICE</v>
-          </cell>
-          <cell r="G19">
-            <v>38.647544558124402</v>
-          </cell>
-          <cell r="H19">
-            <v>38.647544505439768</v>
-          </cell>
-          <cell r="I19">
-            <v>38.647544645524597</v>
-          </cell>
-          <cell r="J19">
-            <v>38.647544383625231</v>
-          </cell>
-          <cell r="K19">
-            <v>38.647544562117609</v>
-          </cell>
-          <cell r="L19">
-            <v>38.647544328371573</v>
-          </cell>
-          <cell r="M19">
-            <v>38.647538364410046</v>
-          </cell>
-          <cell r="N19">
-            <v>38.647532379989407</v>
-          </cell>
-          <cell r="O19">
-            <v>38.647536489743565</v>
-          </cell>
-          <cell r="P19">
-            <v>38.647537590620246</v>
-          </cell>
-          <cell r="Q19">
-            <v>38.647532447156081</v>
-          </cell>
-          <cell r="R19">
-            <v>38.647541819225708</v>
           </cell>
         </row>
         <row r="20">
@@ -6154,21 +5101,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1399EC-A8AD-491E-8CBF-A80BA9B0B353}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103DF7E6-4D3C-405A-9F8E-2718AFE29276}">
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:X7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6242,7 +5189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -6298,7 +5245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -6315,7 +5262,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -6332,7 +5279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -6354,52 +5301,52 @@
       <c r="L6" t="s">
         <v>26</v>
       </c>
-      <c r="M6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(M$2,[1]!pyCIMS_year,0))</f>
+      <c r="M6" cm="1">
+        <f t="array" ref="M6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(M$2,[1]!CIMS_year))</f>
         <v>3004198</v>
       </c>
-      <c r="N6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(N$2,[1]!pyCIMS_year,0))</f>
+      <c r="N6" cm="1">
+        <f t="array" ref="N6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(N$2,[1]!CIMS_year))</f>
         <v>3321768</v>
       </c>
-      <c r="O6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(O$2,[1]!pyCIMS_year,0))</f>
+      <c r="O6" cm="1">
+        <f t="array" ref="O6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(O$2,[1]!CIMS_year))</f>
         <v>3732082</v>
       </c>
-      <c r="P6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(P$2,[1]!pyCIMS_year,0))</f>
+      <c r="P6" cm="1">
+        <f t="array" ref="P6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(P$2,[1]!CIMS_year))</f>
         <v>4144491</v>
       </c>
-      <c r="Q6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(Q$2,[1]!pyCIMS_year,0))</f>
+      <c r="Q6" cm="1">
+        <f t="array" ref="Q6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(Q$2,[1]!CIMS_year))</f>
         <v>4420029</v>
       </c>
-      <c r="R6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(R$2,[1]!pyCIMS_year,0))</f>
+      <c r="R6" cm="1">
+        <f t="array" ref="R6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(R$2,[1]!CIMS_year))</f>
         <v>4965000</v>
       </c>
-      <c r="S6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(S$2,[1]!pyCIMS_year,0))</f>
+      <c r="S6" cm="1">
+        <f t="array" ref="S6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(S$2,[1]!CIMS_year))</f>
         <v>5460100</v>
       </c>
-      <c r="T6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(T$2,[1]!pyCIMS_year,0))</f>
+      <c r="T6" cm="1">
+        <f t="array" ref="T6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(T$2,[1]!CIMS_year))</f>
         <v>5976700</v>
       </c>
-      <c r="U6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(U$2,[1]!pyCIMS_year,0))</f>
+      <c r="U6" cm="1">
+        <f t="array" ref="U6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(U$2,[1]!CIMS_year))</f>
         <v>6515600</v>
       </c>
-      <c r="V6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(V$2,[1]!pyCIMS_year,0))</f>
+      <c r="V6" cm="1">
+        <f t="array" ref="V6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(V$2,[1]!CIMS_year))</f>
         <v>6751778.2937559607</v>
       </c>
-      <c r="W6">
-        <f ca="1">INDEX([1]!pyCIMS_population,MATCH($C6,[1]!region_CIMS,0),MATCH(W$2,[1]!pyCIMS_year,0))</f>
+      <c r="W6" cm="1">
+        <f t="array" ref="W6">INDEX([1]!CIMS_population,_xlfn.XMATCH($C6,[1]!region_CIMS),_xlfn.XMATCH(W$2,[1]!CIMS_year))</f>
         <v>6981842.726861191</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -6421,48 +5368,48 @@
       <c r="L7" t="s">
         <v>28</v>
       </c>
-      <c r="M7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(M$2,[1]!pyCIMS_year,0))</f>
+      <c r="M7" cm="1">
+        <f t="array" ref="M7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(M$2,[1]!CIMS_year))</f>
         <v>241251.75158053398</v>
       </c>
-      <c r="N7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(N$2,[1]!pyCIMS_year,0))</f>
+      <c r="N7" cm="1">
+        <f t="array" ref="N7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(N$2,[1]!CIMS_year))</f>
         <v>286047.23224697507</v>
       </c>
-      <c r="O7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(O$2,[1]!pyCIMS_year,0))</f>
+      <c r="O7" cm="1">
+        <f t="array" ref="O7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(O$2,[1]!CIMS_year))</f>
         <v>311884.83832539228</v>
       </c>
-      <c r="P7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(P$2,[1]!pyCIMS_year,0))</f>
+      <c r="P7" cm="1">
+        <f t="array" ref="P7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(P$2,[1]!CIMS_year))</f>
         <v>371864.0496689151</v>
       </c>
-      <c r="Q7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(Q$2,[1]!pyCIMS_year,0))</f>
+      <c r="Q7" cm="1">
+        <f t="array" ref="Q7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(Q$2,[1]!CIMS_year))</f>
         <v>352708.69722059922</v>
       </c>
-      <c r="R7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(R$2,[1]!pyCIMS_year,0))</f>
+      <c r="R7" cm="1">
+        <f t="array" ref="R7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(R$2,[1]!CIMS_year))</f>
         <v>398094.70776005066</v>
       </c>
-      <c r="S7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(S$2,[1]!pyCIMS_year,0))</f>
+      <c r="S7" cm="1">
+        <f t="array" ref="S7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(S$2,[1]!CIMS_year))</f>
         <v>440960.56814001396</v>
       </c>
-      <c r="T7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(T$2,[1]!pyCIMS_year,0))</f>
+      <c r="T7" cm="1">
+        <f t="array" ref="T7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(T$2,[1]!CIMS_year))</f>
         <v>484955.42138564883</v>
       </c>
-      <c r="U7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(U$2,[1]!pyCIMS_year,0))</f>
+      <c r="U7" cm="1">
+        <f t="array" ref="U7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(U$2,[1]!CIMS_year))</f>
         <v>535701.75694266777</v>
       </c>
-      <c r="V7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(V$2,[1]!pyCIMS_year,0))</f>
+      <c r="V7" cm="1">
+        <f t="array" ref="V7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(V$2,[1]!CIMS_year))</f>
         <v>591527.46226970514</v>
       </c>
-      <c r="W7">
-        <f ca="1">INDEX([1]!pyCIMS_GDP,MATCH($C7,[1]!region_CIMS,0),MATCH(W$2,[1]!pyCIMS_year,0))</f>
+      <c r="W7" cm="1">
+        <f t="array" ref="W7">INDEX([1]!CIMS_GDP,_xlfn.XMATCH($C7,[1]!region_CIMS),_xlfn.XMATCH(W$2,[1]!CIMS_year))</f>
         <v>650318.67160160968</v>
       </c>
     </row>

</xml_diff>